<commit_message>
Moving towards legacy support
</commit_message>
<xml_diff>
--- a/forms/Form-1DI.xlsx
+++ b/forms/Form-1DI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\Data dissemination\iotc-reference-data\forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10258E5-0F0D-40F6-90C9-40E9B7D8C55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CF8A0B-34B7-454A-986C-1BEE2B12C912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Focal point</t>
   </si>
@@ -120,9 +120,6 @@
     <t>IOTC form 1-DI | data</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>Data raising</t>
   </si>
   <si>
@@ -142,6 +139,12 @@
   </si>
   <si>
     <t>Catch unit</t>
+  </si>
+  <si>
+    <t>1.0.0-legacy</t>
+  </si>
+  <si>
+    <t>Target species</t>
   </si>
 </sst>
 </file>
@@ -1465,7 +1468,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1620,7 +1623,7 @@
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="79" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="47"/>
       <c r="E19" s="10"/>
@@ -1700,7 +1703,7 @@
       <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="m/TJ+H8Hy2DjroJT9Lyp2/148I9Hvxx7aq16lekEylHgWGycwNrbD5tkLdHeb7CmjT7weFuH9ZWJ9coDfiji2g==" saltValue="JraXn1XBMh++x0FLAr//kA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rtuR/uOoHr+r8AYA+5yXx9aiAvELAOGvXdZyjSve7v9g6W5VUcJf2qALb9VAtzcdAkLwpyc7bhCXv/PqaBk2Eg==" saltValue="Rz9FRYGiKrhzcHd3RoVoCQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C8:D8"/>
@@ -1723,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BI1048575"/>
+  <dimension ref="A1:BJ1048575"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <pane xSplit="11" ySplit="7" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="7" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
@@ -1736,25 +1739,25 @@
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="52" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="48" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="48" customWidth="1"/>
-    <col min="5" max="5" width="14" style="69" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="52" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="48" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="56" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="52" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="60" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="66" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="62"/>
-    <col min="13" max="60" width="9.140625" style="48"/>
-    <col min="61" max="61" width="9.140625" style="56"/>
-    <col min="62" max="16384" width="9.140625" style="25"/>
+    <col min="3" max="4" width="15.7109375" style="48" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="48" customWidth="1"/>
+    <col min="6" max="6" width="14" style="69" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="52" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="48" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="56" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="52" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="60" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="66" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="62"/>
+    <col min="14" max="61" width="9.140625" style="48"/>
+    <col min="62" max="62" width="9.140625" style="56"/>
+    <col min="63" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J1" s="42"/>
-    </row>
-    <row r="2" spans="1:61" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:62" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="42"/>
+    </row>
+    <row r="2" spans="1:62" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="85" t="s">
         <v>26</v>
       </c>
@@ -1766,8 +1769,8 @@
       <c r="H2" s="86"/>
       <c r="I2" s="86"/>
       <c r="J2" s="86"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="38"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="112"/>
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
       <c r="O2" s="38"/>
@@ -1816,9 +1819,10 @@
       <c r="BF2" s="38"/>
       <c r="BG2" s="38"/>
       <c r="BH2" s="38"/>
-      <c r="BI2" s="39"/>
-    </row>
-    <row r="3" spans="1:61" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BI2" s="38"/>
+      <c r="BJ2" s="39"/>
+    </row>
+    <row r="3" spans="1:62" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40"/>
       <c r="B3" s="88"/>
       <c r="C3" s="89"/>
@@ -1829,11 +1833,11 @@
       <c r="H3" s="89"/>
       <c r="I3" s="89"/>
       <c r="J3" s="89"/>
-      <c r="K3" s="113"/>
-      <c r="L3" s="109" t="s">
+      <c r="K3" s="89"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="110"/>
       <c r="N3" s="110"/>
       <c r="O3" s="110"/>
       <c r="P3" s="110"/>
@@ -1881,29 +1885,30 @@
       <c r="BF3" s="110"/>
       <c r="BG3" s="110"/>
       <c r="BH3" s="110"/>
-      <c r="BI3" s="111"/>
-    </row>
-    <row r="4" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI3" s="110"/>
+      <c r="BJ3" s="111"/>
+    </row>
+    <row r="4" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="91" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="92"/>
       <c r="D4" s="92"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="100" t="s">
+      <c r="E4" s="92"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="101"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="100" t="s">
+      <c r="H4" s="101"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="102"/>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="102"/>
+      <c r="L4" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
+      <c r="M4" s="26"/>
       <c r="N4" s="27"/>
       <c r="O4" s="27"/>
       <c r="P4" s="27"/>
@@ -1951,23 +1956,24 @@
       <c r="BF4" s="27"/>
       <c r="BG4" s="27"/>
       <c r="BH4" s="27"/>
-      <c r="BI4" s="28"/>
-    </row>
-    <row r="5" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BI4" s="27"/>
+      <c r="BJ4" s="28"/>
+    </row>
+    <row r="5" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="94"/>
       <c r="C5" s="95"/>
       <c r="D5" s="95"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="76" t="s">
+      <c r="E5" s="95"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="27"/>
+      <c r="M5" s="26"/>
       <c r="N5" s="27"/>
       <c r="O5" s="27"/>
       <c r="P5" s="27"/>
@@ -2015,23 +2021,24 @@
       <c r="BF5" s="27"/>
       <c r="BG5" s="27"/>
       <c r="BH5" s="27"/>
-      <c r="BI5" s="28"/>
-    </row>
-    <row r="6" spans="1:61" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BI5" s="27"/>
+      <c r="BJ5" s="28"/>
+    </row>
+    <row r="6" spans="1:62" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="97"/>
       <c r="C6" s="98"/>
       <c r="D6" s="98"/>
-      <c r="E6" s="99"/>
-      <c r="F6" s="106"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="108"/>
-      <c r="K6" s="46" t="s">
-        <v>28</v>
+      <c r="E6" s="98"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="46" t="s">
+        <v>27</v>
       </c>
-      <c r="L6" s="26"/>
-      <c r="M6" s="27"/>
+      <c r="M6" s="26"/>
       <c r="N6" s="27"/>
       <c r="O6" s="27"/>
       <c r="P6" s="27"/>
@@ -2079,41 +2086,44 @@
       <c r="BF6" s="27"/>
       <c r="BG6" s="27"/>
       <c r="BH6" s="27"/>
-      <c r="BI6" s="28"/>
-    </row>
-    <row r="7" spans="1:61" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BI6" s="27"/>
+      <c r="BJ6" s="28"/>
+    </row>
+    <row r="7" spans="1:62" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="41" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="71" t="s">
-        <v>31</v>
+      <c r="D7" s="70" t="s">
+        <v>35</v>
       </c>
-      <c r="E7" s="72" t="s">
+      <c r="E7" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="72" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="74" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="29"/>
-      <c r="M7" s="30"/>
+      <c r="M7" s="29"/>
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
       <c r="P7" s="30"/>
@@ -2161,21 +2171,22 @@
       <c r="BF7" s="30"/>
       <c r="BG7" s="30"/>
       <c r="BH7" s="30"/>
-      <c r="BI7" s="31"/>
-    </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BI7" s="30"/>
+      <c r="BJ7" s="31"/>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B8" s="49"/>
       <c r="C8" s="50"/>
       <c r="D8" s="50"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="63"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="57"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="61"/>
       <c r="N8" s="57"/>
       <c r="O8" s="57"/>
       <c r="P8" s="57"/>
@@ -2223,21 +2234,22 @@
       <c r="BF8" s="57"/>
       <c r="BG8" s="57"/>
       <c r="BH8" s="57"/>
-      <c r="BI8" s="58"/>
-    </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BI8" s="57"/>
+      <c r="BJ8" s="58"/>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="36"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="35"/>
       <c r="N9" s="36"/>
       <c r="O9" s="36"/>
       <c r="P9" s="36"/>
@@ -2285,21 +2297,22 @@
       <c r="BF9" s="36"/>
       <c r="BG9" s="36"/>
       <c r="BH9" s="36"/>
-      <c r="BI9" s="37"/>
-    </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BI9" s="36"/>
+      <c r="BJ9" s="37"/>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="55"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="36"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="35"/>
       <c r="N10" s="36"/>
       <c r="O10" s="36"/>
       <c r="P10" s="36"/>
@@ -2347,21 +2360,22 @@
       <c r="BF10" s="36"/>
       <c r="BG10" s="36"/>
       <c r="BH10" s="36"/>
-      <c r="BI10" s="37"/>
-    </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BI10" s="36"/>
+      <c r="BJ10" s="37"/>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B11" s="32"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="36"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="35"/>
       <c r="N11" s="36"/>
       <c r="O11" s="36"/>
       <c r="P11" s="36"/>
@@ -2409,21 +2423,22 @@
       <c r="BF11" s="36"/>
       <c r="BG11" s="36"/>
       <c r="BH11" s="36"/>
-      <c r="BI11" s="37"/>
-    </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BI11" s="36"/>
+      <c r="BJ11" s="37"/>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B12" s="32"/>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="36"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="35"/>
       <c r="N12" s="36"/>
       <c r="O12" s="36"/>
       <c r="P12" s="36"/>
@@ -2471,21 +2486,22 @@
       <c r="BF12" s="36"/>
       <c r="BG12" s="36"/>
       <c r="BH12" s="36"/>
-      <c r="BI12" s="37"/>
-    </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BI12" s="36"/>
+      <c r="BJ12" s="37"/>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B13" s="32"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="36"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="35"/>
       <c r="N13" s="36"/>
       <c r="O13" s="36"/>
       <c r="P13" s="36"/>
@@ -2533,21 +2549,22 @@
       <c r="BF13" s="36"/>
       <c r="BG13" s="36"/>
       <c r="BH13" s="36"/>
-      <c r="BI13" s="37"/>
-    </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BI13" s="36"/>
+      <c r="BJ13" s="37"/>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="36"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="35"/>
       <c r="N14" s="36"/>
       <c r="O14" s="36"/>
       <c r="P14" s="36"/>
@@ -2595,21 +2612,22 @@
       <c r="BF14" s="36"/>
       <c r="BG14" s="36"/>
       <c r="BH14" s="36"/>
-      <c r="BI14" s="37"/>
-    </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BI14" s="36"/>
+      <c r="BJ14" s="37"/>
+    </row>
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B15" s="32"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="36"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="35"/>
       <c r="N15" s="36"/>
       <c r="O15" s="36"/>
       <c r="P15" s="36"/>
@@ -2657,21 +2675,22 @@
       <c r="BF15" s="36"/>
       <c r="BG15" s="36"/>
       <c r="BH15" s="36"/>
-      <c r="BI15" s="37"/>
-    </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="BI15" s="36"/>
+      <c r="BJ15" s="37"/>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="B16" s="32"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="36"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="35"/>
       <c r="N16" s="36"/>
       <c r="O16" s="36"/>
       <c r="P16" s="36"/>
@@ -2719,21 +2738,22 @@
       <c r="BF16" s="36"/>
       <c r="BG16" s="36"/>
       <c r="BH16" s="36"/>
-      <c r="BI16" s="37"/>
-    </row>
-    <row r="17" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI16" s="36"/>
+      <c r="BJ16" s="37"/>
+    </row>
+    <row r="17" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B17" s="32"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="36"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="36"/>
       <c r="O17" s="36"/>
       <c r="P17" s="36"/>
@@ -2781,21 +2801,22 @@
       <c r="BF17" s="36"/>
       <c r="BG17" s="36"/>
       <c r="BH17" s="36"/>
-      <c r="BI17" s="37"/>
-    </row>
-    <row r="18" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI17" s="36"/>
+      <c r="BJ17" s="37"/>
+    </row>
+    <row r="18" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="35"/>
       <c r="N18" s="36"/>
       <c r="O18" s="36"/>
       <c r="P18" s="36"/>
@@ -2843,21 +2864,22 @@
       <c r="BF18" s="36"/>
       <c r="BG18" s="36"/>
       <c r="BH18" s="36"/>
-      <c r="BI18" s="37"/>
-    </row>
-    <row r="19" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI18" s="36"/>
+      <c r="BJ18" s="37"/>
+    </row>
+    <row r="19" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="36"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="36"/>
       <c r="O19" s="36"/>
       <c r="P19" s="36"/>
@@ -2905,21 +2927,22 @@
       <c r="BF19" s="36"/>
       <c r="BG19" s="36"/>
       <c r="BH19" s="36"/>
-      <c r="BI19" s="37"/>
-    </row>
-    <row r="20" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI19" s="36"/>
+      <c r="BJ19" s="37"/>
+    </row>
+    <row r="20" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="36"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="35"/>
       <c r="N20" s="36"/>
       <c r="O20" s="36"/>
       <c r="P20" s="36"/>
@@ -2967,21 +2990,22 @@
       <c r="BF20" s="36"/>
       <c r="BG20" s="36"/>
       <c r="BH20" s="36"/>
-      <c r="BI20" s="37"/>
-    </row>
-    <row r="21" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI20" s="36"/>
+      <c r="BJ20" s="37"/>
+    </row>
+    <row r="21" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="36"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="35"/>
       <c r="N21" s="36"/>
       <c r="O21" s="36"/>
       <c r="P21" s="36"/>
@@ -3029,21 +3053,22 @@
       <c r="BF21" s="36"/>
       <c r="BG21" s="36"/>
       <c r="BH21" s="36"/>
-      <c r="BI21" s="37"/>
-    </row>
-    <row r="22" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI21" s="36"/>
+      <c r="BJ21" s="37"/>
+    </row>
+    <row r="22" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="64"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="36"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="35"/>
       <c r="N22" s="36"/>
       <c r="O22" s="36"/>
       <c r="P22" s="36"/>
@@ -3091,21 +3116,22 @@
       <c r="BF22" s="36"/>
       <c r="BG22" s="36"/>
       <c r="BH22" s="36"/>
-      <c r="BI22" s="37"/>
-    </row>
-    <row r="23" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI22" s="36"/>
+      <c r="BJ22" s="37"/>
+    </row>
+    <row r="23" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
-      <c r="E23" s="68"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="36"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="35"/>
       <c r="N23" s="36"/>
       <c r="O23" s="36"/>
       <c r="P23" s="36"/>
@@ -3153,21 +3179,22 @@
       <c r="BF23" s="36"/>
       <c r="BG23" s="36"/>
       <c r="BH23" s="36"/>
-      <c r="BI23" s="37"/>
-    </row>
-    <row r="24" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI23" s="36"/>
+      <c r="BJ23" s="37"/>
+    </row>
+    <row r="24" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B24" s="32"/>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="36"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="35"/>
       <c r="N24" s="36"/>
       <c r="O24" s="36"/>
       <c r="P24" s="36"/>
@@ -3215,21 +3242,22 @@
       <c r="BF24" s="36"/>
       <c r="BG24" s="36"/>
       <c r="BH24" s="36"/>
-      <c r="BI24" s="37"/>
-    </row>
-    <row r="25" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI24" s="36"/>
+      <c r="BJ24" s="37"/>
+    </row>
+    <row r="25" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B25" s="32"/>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="36"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="34"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="35"/>
       <c r="N25" s="36"/>
       <c r="O25" s="36"/>
       <c r="P25" s="36"/>
@@ -3277,21 +3305,22 @@
       <c r="BF25" s="36"/>
       <c r="BG25" s="36"/>
       <c r="BH25" s="36"/>
-      <c r="BI25" s="37"/>
-    </row>
-    <row r="26" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI25" s="36"/>
+      <c r="BJ25" s="37"/>
+    </row>
+    <row r="26" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="36"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="35"/>
       <c r="N26" s="36"/>
       <c r="O26" s="36"/>
       <c r="P26" s="36"/>
@@ -3339,21 +3368,22 @@
       <c r="BF26" s="36"/>
       <c r="BG26" s="36"/>
       <c r="BH26" s="36"/>
-      <c r="BI26" s="37"/>
-    </row>
-    <row r="27" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI26" s="36"/>
+      <c r="BJ26" s="37"/>
+    </row>
+    <row r="27" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B27" s="32"/>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="43"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="36"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="35"/>
       <c r="N27" s="36"/>
       <c r="O27" s="36"/>
       <c r="P27" s="36"/>
@@ -3401,21 +3431,22 @@
       <c r="BF27" s="36"/>
       <c r="BG27" s="36"/>
       <c r="BH27" s="36"/>
-      <c r="BI27" s="37"/>
-    </row>
-    <row r="28" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI27" s="36"/>
+      <c r="BJ27" s="37"/>
+    </row>
+    <row r="28" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="35"/>
-      <c r="M28" s="36"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="43"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="35"/>
       <c r="N28" s="36"/>
       <c r="O28" s="36"/>
       <c r="P28" s="36"/>
@@ -3463,21 +3494,22 @@
       <c r="BF28" s="36"/>
       <c r="BG28" s="36"/>
       <c r="BH28" s="36"/>
-      <c r="BI28" s="37"/>
-    </row>
-    <row r="29" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI28" s="36"/>
+      <c r="BJ28" s="37"/>
+    </row>
+    <row r="29" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B29" s="32"/>
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="34"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="36"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="35"/>
       <c r="N29" s="36"/>
       <c r="O29" s="36"/>
       <c r="P29" s="36"/>
@@ -3525,21 +3557,22 @@
       <c r="BF29" s="36"/>
       <c r="BG29" s="36"/>
       <c r="BH29" s="36"/>
-      <c r="BI29" s="37"/>
-    </row>
-    <row r="30" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI29" s="36"/>
+      <c r="BJ29" s="37"/>
+    </row>
+    <row r="30" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="35"/>
-      <c r="M30" s="36"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="55"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="35"/>
       <c r="N30" s="36"/>
       <c r="O30" s="36"/>
       <c r="P30" s="36"/>
@@ -3587,21 +3620,22 @@
       <c r="BF30" s="36"/>
       <c r="BG30" s="36"/>
       <c r="BH30" s="36"/>
-      <c r="BI30" s="37"/>
-    </row>
-    <row r="31" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI30" s="36"/>
+      <c r="BJ30" s="37"/>
+    </row>
+    <row r="31" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B31" s="32"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="64"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="36"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="35"/>
       <c r="N31" s="36"/>
       <c r="O31" s="36"/>
       <c r="P31" s="36"/>
@@ -3649,21 +3683,22 @@
       <c r="BF31" s="36"/>
       <c r="BG31" s="36"/>
       <c r="BH31" s="36"/>
-      <c r="BI31" s="37"/>
-    </row>
-    <row r="32" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI31" s="36"/>
+      <c r="BJ31" s="37"/>
+    </row>
+    <row r="32" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="55"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="36"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="35"/>
       <c r="N32" s="36"/>
       <c r="O32" s="36"/>
       <c r="P32" s="36"/>
@@ -3711,21 +3746,22 @@
       <c r="BF32" s="36"/>
       <c r="BG32" s="36"/>
       <c r="BH32" s="36"/>
-      <c r="BI32" s="37"/>
-    </row>
-    <row r="33" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI32" s="36"/>
+      <c r="BJ32" s="37"/>
+    </row>
+    <row r="33" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="55"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="36"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="35"/>
       <c r="N33" s="36"/>
       <c r="O33" s="36"/>
       <c r="P33" s="36"/>
@@ -3773,21 +3809,22 @@
       <c r="BF33" s="36"/>
       <c r="BG33" s="36"/>
       <c r="BH33" s="36"/>
-      <c r="BI33" s="37"/>
-    </row>
-    <row r="34" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI33" s="36"/>
+      <c r="BJ33" s="37"/>
+    </row>
+    <row r="34" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B34" s="32"/>
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="36"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="35"/>
       <c r="N34" s="36"/>
       <c r="O34" s="36"/>
       <c r="P34" s="36"/>
@@ -3835,21 +3872,22 @@
       <c r="BF34" s="36"/>
       <c r="BG34" s="36"/>
       <c r="BH34" s="36"/>
-      <c r="BI34" s="37"/>
-    </row>
-    <row r="35" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI34" s="36"/>
+      <c r="BJ34" s="37"/>
+    </row>
+    <row r="35" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B35" s="32"/>
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="64"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="36"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="35"/>
       <c r="N35" s="36"/>
       <c r="O35" s="36"/>
       <c r="P35" s="36"/>
@@ -3897,21 +3935,22 @@
       <c r="BF35" s="36"/>
       <c r="BG35" s="36"/>
       <c r="BH35" s="36"/>
-      <c r="BI35" s="37"/>
-    </row>
-    <row r="36" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI35" s="36"/>
+      <c r="BJ35" s="37"/>
+    </row>
+    <row r="36" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
-      <c r="E36" s="68"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="34"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="64"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="36"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="35"/>
       <c r="N36" s="36"/>
       <c r="O36" s="36"/>
       <c r="P36" s="36"/>
@@ -3959,21 +3998,22 @@
       <c r="BF36" s="36"/>
       <c r="BG36" s="36"/>
       <c r="BH36" s="36"/>
-      <c r="BI36" s="37"/>
-    </row>
-    <row r="37" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI36" s="36"/>
+      <c r="BJ36" s="37"/>
+    </row>
+    <row r="37" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B37" s="32"/>
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="64"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="36"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="64"/>
+      <c r="M37" s="35"/>
       <c r="N37" s="36"/>
       <c r="O37" s="36"/>
       <c r="P37" s="36"/>
@@ -4021,21 +4061,22 @@
       <c r="BF37" s="36"/>
       <c r="BG37" s="36"/>
       <c r="BH37" s="36"/>
-      <c r="BI37" s="37"/>
-    </row>
-    <row r="38" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI37" s="36"/>
+      <c r="BJ37" s="37"/>
+    </row>
+    <row r="38" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B38" s="32"/>
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
-      <c r="E38" s="68"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="43"/>
-      <c r="K38" s="64"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="36"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="64"/>
+      <c r="M38" s="35"/>
       <c r="N38" s="36"/>
       <c r="O38" s="36"/>
       <c r="P38" s="36"/>
@@ -4083,21 +4124,22 @@
       <c r="BF38" s="36"/>
       <c r="BG38" s="36"/>
       <c r="BH38" s="36"/>
-      <c r="BI38" s="37"/>
-    </row>
-    <row r="39" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI38" s="36"/>
+      <c r="BJ38" s="37"/>
+    </row>
+    <row r="39" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B39" s="32"/>
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
-      <c r="E39" s="68"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="55"/>
-      <c r="J39" s="43"/>
-      <c r="K39" s="64"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="36"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="68"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="35"/>
       <c r="N39" s="36"/>
       <c r="O39" s="36"/>
       <c r="P39" s="36"/>
@@ -4145,21 +4187,22 @@
       <c r="BF39" s="36"/>
       <c r="BG39" s="36"/>
       <c r="BH39" s="36"/>
-      <c r="BI39" s="37"/>
-    </row>
-    <row r="40" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI39" s="36"/>
+      <c r="BJ39" s="37"/>
+    </row>
+    <row r="40" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B40" s="32"/>
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
-      <c r="E40" s="68"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="64"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="36"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="43"/>
+      <c r="L40" s="64"/>
+      <c r="M40" s="35"/>
       <c r="N40" s="36"/>
       <c r="O40" s="36"/>
       <c r="P40" s="36"/>
@@ -4207,21 +4250,22 @@
       <c r="BF40" s="36"/>
       <c r="BG40" s="36"/>
       <c r="BH40" s="36"/>
-      <c r="BI40" s="37"/>
-    </row>
-    <row r="41" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI40" s="36"/>
+      <c r="BJ40" s="37"/>
+    </row>
+    <row r="41" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B41" s="32"/>
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="64"/>
-      <c r="L41" s="35"/>
-      <c r="M41" s="36"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="64"/>
+      <c r="M41" s="35"/>
       <c r="N41" s="36"/>
       <c r="O41" s="36"/>
       <c r="P41" s="36"/>
@@ -4269,21 +4313,22 @@
       <c r="BF41" s="36"/>
       <c r="BG41" s="36"/>
       <c r="BH41" s="36"/>
-      <c r="BI41" s="37"/>
-    </row>
-    <row r="42" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI41" s="36"/>
+      <c r="BJ41" s="37"/>
+    </row>
+    <row r="42" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B42" s="32"/>
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="34"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="43"/>
-      <c r="K42" s="64"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="36"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="43"/>
+      <c r="L42" s="64"/>
+      <c r="M42" s="35"/>
       <c r="N42" s="36"/>
       <c r="O42" s="36"/>
       <c r="P42" s="36"/>
@@ -4331,21 +4376,22 @@
       <c r="BF42" s="36"/>
       <c r="BG42" s="36"/>
       <c r="BH42" s="36"/>
-      <c r="BI42" s="37"/>
-    </row>
-    <row r="43" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI42" s="36"/>
+      <c r="BJ42" s="37"/>
+    </row>
+    <row r="43" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="55"/>
-      <c r="J43" s="43"/>
-      <c r="K43" s="64"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="36"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="64"/>
+      <c r="M43" s="35"/>
       <c r="N43" s="36"/>
       <c r="O43" s="36"/>
       <c r="P43" s="36"/>
@@ -4393,21 +4439,22 @@
       <c r="BF43" s="36"/>
       <c r="BG43" s="36"/>
       <c r="BH43" s="36"/>
-      <c r="BI43" s="37"/>
-    </row>
-    <row r="44" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI43" s="36"/>
+      <c r="BJ43" s="37"/>
+    </row>
+    <row r="44" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
       <c r="C44" s="33"/>
       <c r="D44" s="33"/>
-      <c r="E44" s="68"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="64"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="36"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="35"/>
       <c r="N44" s="36"/>
       <c r="O44" s="36"/>
       <c r="P44" s="36"/>
@@ -4455,21 +4502,22 @@
       <c r="BF44" s="36"/>
       <c r="BG44" s="36"/>
       <c r="BH44" s="36"/>
-      <c r="BI44" s="37"/>
-    </row>
-    <row r="45" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI44" s="36"/>
+      <c r="BJ44" s="37"/>
+    </row>
+    <row r="45" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
       <c r="C45" s="33"/>
       <c r="D45" s="33"/>
-      <c r="E45" s="68"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="35"/>
-      <c r="M45" s="36"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="64"/>
+      <c r="M45" s="35"/>
       <c r="N45" s="36"/>
       <c r="O45" s="36"/>
       <c r="P45" s="36"/>
@@ -4517,21 +4565,22 @@
       <c r="BF45" s="36"/>
       <c r="BG45" s="36"/>
       <c r="BH45" s="36"/>
-      <c r="BI45" s="37"/>
-    </row>
-    <row r="46" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI45" s="36"/>
+      <c r="BJ45" s="37"/>
+    </row>
+    <row r="46" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B46" s="32"/>
       <c r="C46" s="33"/>
       <c r="D46" s="33"/>
-      <c r="E46" s="68"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="36"/>
+      <c r="E46" s="33"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="43"/>
+      <c r="L46" s="64"/>
+      <c r="M46" s="35"/>
       <c r="N46" s="36"/>
       <c r="O46" s="36"/>
       <c r="P46" s="36"/>
@@ -4579,21 +4628,22 @@
       <c r="BF46" s="36"/>
       <c r="BG46" s="36"/>
       <c r="BH46" s="36"/>
-      <c r="BI46" s="37"/>
-    </row>
-    <row r="47" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI46" s="36"/>
+      <c r="BJ46" s="37"/>
+    </row>
+    <row r="47" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B47" s="32"/>
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
-      <c r="E47" s="68"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="64"/>
-      <c r="L47" s="35"/>
-      <c r="M47" s="36"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="64"/>
+      <c r="M47" s="35"/>
       <c r="N47" s="36"/>
       <c r="O47" s="36"/>
       <c r="P47" s="36"/>
@@ -4641,21 +4691,22 @@
       <c r="BF47" s="36"/>
       <c r="BG47" s="36"/>
       <c r="BH47" s="36"/>
-      <c r="BI47" s="37"/>
-    </row>
-    <row r="48" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI47" s="36"/>
+      <c r="BJ47" s="37"/>
+    </row>
+    <row r="48" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B48" s="32"/>
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
-      <c r="E48" s="68"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="55"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="64"/>
-      <c r="L48" s="35"/>
-      <c r="M48" s="36"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="43"/>
+      <c r="L48" s="64"/>
+      <c r="M48" s="35"/>
       <c r="N48" s="36"/>
       <c r="O48" s="36"/>
       <c r="P48" s="36"/>
@@ -4703,21 +4754,22 @@
       <c r="BF48" s="36"/>
       <c r="BG48" s="36"/>
       <c r="BH48" s="36"/>
-      <c r="BI48" s="37"/>
-    </row>
-    <row r="49" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI48" s="36"/>
+      <c r="BJ48" s="37"/>
+    </row>
+    <row r="49" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B49" s="32"/>
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
-      <c r="E49" s="68"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="55"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="64"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="36"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="68"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="55"/>
+      <c r="K49" s="43"/>
+      <c r="L49" s="64"/>
+      <c r="M49" s="35"/>
       <c r="N49" s="36"/>
       <c r="O49" s="36"/>
       <c r="P49" s="36"/>
@@ -4765,21 +4817,22 @@
       <c r="BF49" s="36"/>
       <c r="BG49" s="36"/>
       <c r="BH49" s="36"/>
-      <c r="BI49" s="37"/>
-    </row>
-    <row r="50" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI49" s="36"/>
+      <c r="BJ49" s="37"/>
+    </row>
+    <row r="50" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B50" s="32"/>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
-      <c r="E50" s="68"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="33"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="64"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="36"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="68"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="43"/>
+      <c r="L50" s="64"/>
+      <c r="M50" s="35"/>
       <c r="N50" s="36"/>
       <c r="O50" s="36"/>
       <c r="P50" s="36"/>
@@ -4827,21 +4880,22 @@
       <c r="BF50" s="36"/>
       <c r="BG50" s="36"/>
       <c r="BH50" s="36"/>
-      <c r="BI50" s="37"/>
-    </row>
-    <row r="51" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI50" s="36"/>
+      <c r="BJ50" s="37"/>
+    </row>
+    <row r="51" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B51" s="32"/>
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="33"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="55"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="64"/>
-      <c r="L51" s="35"/>
-      <c r="M51" s="36"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="68"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="43"/>
+      <c r="L51" s="64"/>
+      <c r="M51" s="35"/>
       <c r="N51" s="36"/>
       <c r="O51" s="36"/>
       <c r="P51" s="36"/>
@@ -4889,21 +4943,22 @@
       <c r="BF51" s="36"/>
       <c r="BG51" s="36"/>
       <c r="BH51" s="36"/>
-      <c r="BI51" s="37"/>
-    </row>
-    <row r="52" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI51" s="36"/>
+      <c r="BJ51" s="37"/>
+    </row>
+    <row r="52" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B52" s="32"/>
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
-      <c r="E52" s="68"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="34"/>
-      <c r="I52" s="55"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="64"/>
-      <c r="L52" s="35"/>
-      <c r="M52" s="36"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="55"/>
+      <c r="K52" s="43"/>
+      <c r="L52" s="64"/>
+      <c r="M52" s="35"/>
       <c r="N52" s="36"/>
       <c r="O52" s="36"/>
       <c r="P52" s="36"/>
@@ -4951,21 +5006,22 @@
       <c r="BF52" s="36"/>
       <c r="BG52" s="36"/>
       <c r="BH52" s="36"/>
-      <c r="BI52" s="37"/>
-    </row>
-    <row r="53" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI52" s="36"/>
+      <c r="BJ52" s="37"/>
+    </row>
+    <row r="53" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B53" s="32"/>
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
-      <c r="E53" s="68"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="43"/>
-      <c r="K53" s="64"/>
-      <c r="L53" s="35"/>
-      <c r="M53" s="36"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="68"/>
+      <c r="G53" s="32"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="55"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="64"/>
+      <c r="M53" s="35"/>
       <c r="N53" s="36"/>
       <c r="O53" s="36"/>
       <c r="P53" s="36"/>
@@ -5013,21 +5069,22 @@
       <c r="BF53" s="36"/>
       <c r="BG53" s="36"/>
       <c r="BH53" s="36"/>
-      <c r="BI53" s="37"/>
-    </row>
-    <row r="54" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI53" s="36"/>
+      <c r="BJ53" s="37"/>
+    </row>
+    <row r="54" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B54" s="32"/>
       <c r="C54" s="33"/>
       <c r="D54" s="33"/>
-      <c r="E54" s="68"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="34"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="43"/>
-      <c r="K54" s="64"/>
-      <c r="L54" s="35"/>
-      <c r="M54" s="36"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="43"/>
+      <c r="L54" s="64"/>
+      <c r="M54" s="35"/>
       <c r="N54" s="36"/>
       <c r="O54" s="36"/>
       <c r="P54" s="36"/>
@@ -5075,21 +5132,22 @@
       <c r="BF54" s="36"/>
       <c r="BG54" s="36"/>
       <c r="BH54" s="36"/>
-      <c r="BI54" s="37"/>
-    </row>
-    <row r="55" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI54" s="36"/>
+      <c r="BJ54" s="37"/>
+    </row>
+    <row r="55" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B55" s="32"/>
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="34"/>
-      <c r="I55" s="55"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="64"/>
-      <c r="L55" s="35"/>
-      <c r="M55" s="36"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="34"/>
+      <c r="J55" s="55"/>
+      <c r="K55" s="43"/>
+      <c r="L55" s="64"/>
+      <c r="M55" s="35"/>
       <c r="N55" s="36"/>
       <c r="O55" s="36"/>
       <c r="P55" s="36"/>
@@ -5137,21 +5195,22 @@
       <c r="BF55" s="36"/>
       <c r="BG55" s="36"/>
       <c r="BH55" s="36"/>
-      <c r="BI55" s="37"/>
-    </row>
-    <row r="56" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI55" s="36"/>
+      <c r="BJ55" s="37"/>
+    </row>
+    <row r="56" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B56" s="32"/>
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
-      <c r="E56" s="68"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="34"/>
-      <c r="I56" s="55"/>
-      <c r="J56" s="43"/>
-      <c r="K56" s="64"/>
-      <c r="L56" s="35"/>
-      <c r="M56" s="36"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="68"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="55"/>
+      <c r="K56" s="43"/>
+      <c r="L56" s="64"/>
+      <c r="M56" s="35"/>
       <c r="N56" s="36"/>
       <c r="O56" s="36"/>
       <c r="P56" s="36"/>
@@ -5199,21 +5258,22 @@
       <c r="BF56" s="36"/>
       <c r="BG56" s="36"/>
       <c r="BH56" s="36"/>
-      <c r="BI56" s="37"/>
-    </row>
-    <row r="57" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="BI56" s="36"/>
+      <c r="BJ56" s="37"/>
+    </row>
+    <row r="57" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B57" s="32"/>
       <c r="C57" s="33"/>
       <c r="D57" s="33"/>
-      <c r="E57" s="68"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="34"/>
-      <c r="I57" s="32"/>
-      <c r="J57" s="43"/>
-      <c r="K57" s="64"/>
-      <c r="L57" s="35"/>
-      <c r="M57" s="36"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="64"/>
+      <c r="M57" s="35"/>
       <c r="N57" s="36"/>
       <c r="O57" s="36"/>
       <c r="P57" s="36"/>
@@ -5261,39 +5321,41 @@
       <c r="BF57" s="36"/>
       <c r="BG57" s="36"/>
       <c r="BH57" s="36"/>
-      <c r="BI57" s="37"/>
-    </row>
-    <row r="1048575" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K1048575" s="65"/>
+      <c r="BI57" s="36"/>
+      <c r="BJ57" s="37"/>
+    </row>
+    <row r="1048575" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L1048575" s="65"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bDJXNMdT5aFfuFfdOQmDGWf24JUQf0d7k/SjsQoLsHnhb1zTLe4J5mYaBanqJILPPaH+VRq6WpxzkwtEKYIUXg==" saltValue="WCxFkeKdBTR4NTS/YqdaqA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wcyjFB+9iTmYhZJZK0XaLx4K6rWCE5N1mPPZVAuBUd5NRmClO+0WZ2FcVxvRYVabavIUNlVkdgiA6Wjyyl/dhQ==" saltValue="jpoFl5ihCsVTqLtmuGe4/g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
-    <mergeCell ref="B4:E6"/>
-    <mergeCell ref="F4:H6"/>
-    <mergeCell ref="I4:J6"/>
-    <mergeCell ref="L3:BI3"/>
-    <mergeCell ref="B2:J3"/>
-    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="B4:F6"/>
+    <mergeCell ref="G4:I6"/>
+    <mergeCell ref="J4:K6"/>
+    <mergeCell ref="M3:BJ3"/>
+    <mergeCell ref="B2:K3"/>
+    <mergeCell ref="L2:L3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:I7 K4:K7" xr:uid="{4028DFA7-3B9E-4D78-9BE4-B9C30D52F4E5}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L7 C7:J7" xr:uid="{4028DFA7-3B9E-4D78-9BE4-B9C30D52F4E5}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" location="IOTCareasMain" xr:uid="{D4A2CA3E-12F1-4D58-9391-D5AB2F74A7F6}"/>
-    <hyperlink ref="F7" r:id="rId2" location="types" xr:uid="{3F41DB2A-0528-4E3B-BBCC-3525F348D05D}"/>
-    <hyperlink ref="G7" r:id="rId3" location="sourcesDI" xr:uid="{87C22EDC-E88B-47B5-A906-5136A2DCB1A3}"/>
-    <hyperlink ref="H7" r:id="rId4" location="processingsDI" xr:uid="{5D715338-F6EA-4526-A9D0-7C9B67DA75F5}"/>
-    <hyperlink ref="I7" r:id="rId5" location="coverageTypes" xr:uid="{FCADF32B-4240-49F8-9CD4-8D05AA29176A}"/>
-    <hyperlink ref="K7" r:id="rId6" location="catchUnits" display="Discard unit" xr:uid="{8E2457EF-BFD9-4480-93F6-844FC19CD52F}"/>
+    <hyperlink ref="E7" r:id="rId1" location="IOTCareasMain" xr:uid="{D4A2CA3E-12F1-4D58-9391-D5AB2F74A7F6}"/>
+    <hyperlink ref="G7" r:id="rId2" location="types" xr:uid="{3F41DB2A-0528-4E3B-BBCC-3525F348D05D}"/>
+    <hyperlink ref="H7" r:id="rId3" location="sourcesDI" xr:uid="{87C22EDC-E88B-47B5-A906-5136A2DCB1A3}"/>
+    <hyperlink ref="I7" r:id="rId4" location="processingsDI" xr:uid="{5D715338-F6EA-4526-A9D0-7C9B67DA75F5}"/>
+    <hyperlink ref="J7" r:id="rId5" location="coverageTypes" xr:uid="{FCADF32B-4240-49F8-9CD4-8D05AA29176A}"/>
+    <hyperlink ref="L7" r:id="rId6" location="catchUnits" display="Discard unit" xr:uid="{8E2457EF-BFD9-4480-93F6-844FC19CD52F}"/>
     <hyperlink ref="C7" r:id="rId7" location="fisheries" xr:uid="{F95149BA-1BB2-46CC-A86F-36B6AC4AFBA6}"/>
-    <hyperlink ref="E7" r:id="rId8" location="discardReasons" display="Disc. reason" xr:uid="{4B127CA8-AB4F-43B9-B5B8-5A77A85A9028}"/>
-    <hyperlink ref="K4" r:id="rId9" location="species" xr:uid="{0BBE03AC-0AAA-41DA-99E5-9DD325DC155B}"/>
-    <hyperlink ref="K5" r:id="rId10" location="catchUnits" display="Discard unit" xr:uid="{431CFE87-EEB6-4BEC-9E8B-1A482800044E}"/>
+    <hyperlink ref="F7" r:id="rId8" location="discardReasons" display="Disc. reason" xr:uid="{4B127CA8-AB4F-43B9-B5B8-5A77A85A9028}"/>
+    <hyperlink ref="L4" r:id="rId9" location="species" xr:uid="{0BBE03AC-0AAA-41DA-99E5-9DD325DC155B}"/>
+    <hyperlink ref="L5" r:id="rId10" location="catchUnits" display="Discard unit" xr:uid="{431CFE87-EEB6-4BEC-9E8B-1A482800044E}"/>
+    <hyperlink ref="D7" r:id="rId11" location="species" xr:uid="{6FA0C96E-7F47-464A-B5AC-18A928C06AB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding conditional validation to cells
</commit_message>
<xml_diff>
--- a/forms/Form-1DI.xlsx
+++ b/forms/Form-1DI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A851C286-73A5-4789-8C87-BDDF4950A1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283B22F3-39A2-4F16-AB24-05A96F5ECBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -259,9 +259,8 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
+      <patternFill patternType="lightDown">
+        <bgColor theme="0" tint="-0.14996795556505021"/>
       </patternFill>
     </fill>
   </fills>
@@ -992,144 +991,159 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1457,24 +1471,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="87"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="90"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="88"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -1524,15 +1538,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="84"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="84" t="s">
+      <c r="F8" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="84"/>
+      <c r="G8" s="82"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1703,11 +1717,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="83"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="81"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1768,10 +1782,10 @@
     <col min="9" max="9" width="11.42578125" style="69" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="66" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" style="72" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="74" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="78"/>
-    <col min="14" max="111" width="9.140625" style="79"/>
-    <col min="112" max="112" width="9.140625" style="80"/>
+    <col min="12" max="12" width="12.140625" style="113" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="76"/>
+    <col min="14" max="111" width="9.140625" style="77"/>
+    <col min="112" max="112" width="9.140625" style="78"/>
     <col min="113" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
@@ -1779,19 +1793,19 @@
       <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:112" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="112"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="110"/>
       <c r="M2" s="35"/>
       <c r="N2" s="35"/>
       <c r="O2" s="35"/>
@@ -1895,137 +1909,137 @@
     </row>
     <row r="3" spans="1:112" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="113"/>
-      <c r="M3" s="109" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="111"/>
+      <c r="M3" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="110"/>
-      <c r="O3" s="110"/>
-      <c r="P3" s="110"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="110"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="110"/>
-      <c r="U3" s="110"/>
-      <c r="V3" s="110"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="110"/>
-      <c r="Y3" s="110"/>
-      <c r="Z3" s="110"/>
-      <c r="AA3" s="110"/>
-      <c r="AB3" s="110"/>
-      <c r="AC3" s="110"/>
-      <c r="AD3" s="110"/>
-      <c r="AE3" s="110"/>
-      <c r="AF3" s="110"/>
-      <c r="AG3" s="110"/>
-      <c r="AH3" s="110"/>
-      <c r="AI3" s="110"/>
-      <c r="AJ3" s="110"/>
-      <c r="AK3" s="110"/>
-      <c r="AL3" s="110"/>
-      <c r="AM3" s="110"/>
-      <c r="AN3" s="110"/>
-      <c r="AO3" s="110"/>
-      <c r="AP3" s="110"/>
-      <c r="AQ3" s="110"/>
-      <c r="AR3" s="110"/>
-      <c r="AS3" s="110"/>
-      <c r="AT3" s="110"/>
-      <c r="AU3" s="110"/>
-      <c r="AV3" s="110"/>
-      <c r="AW3" s="110"/>
-      <c r="AX3" s="110"/>
-      <c r="AY3" s="110"/>
-      <c r="AZ3" s="110"/>
-      <c r="BA3" s="110"/>
-      <c r="BB3" s="110"/>
-      <c r="BC3" s="110"/>
-      <c r="BD3" s="110"/>
-      <c r="BE3" s="110"/>
-      <c r="BF3" s="110"/>
-      <c r="BG3" s="110"/>
-      <c r="BH3" s="110"/>
-      <c r="BI3" s="110"/>
-      <c r="BJ3" s="110"/>
-      <c r="BK3" s="110"/>
-      <c r="BL3" s="110"/>
-      <c r="BM3" s="110"/>
-      <c r="BN3" s="110"/>
-      <c r="BO3" s="110"/>
-      <c r="BP3" s="110"/>
-      <c r="BQ3" s="110"/>
-      <c r="BR3" s="110"/>
-      <c r="BS3" s="110"/>
-      <c r="BT3" s="110"/>
-      <c r="BU3" s="110"/>
-      <c r="BV3" s="110"/>
-      <c r="BW3" s="110"/>
-      <c r="BX3" s="110"/>
-      <c r="BY3" s="110"/>
-      <c r="BZ3" s="110"/>
-      <c r="CA3" s="110"/>
-      <c r="CB3" s="110"/>
-      <c r="CC3" s="110"/>
-      <c r="CD3" s="110"/>
-      <c r="CE3" s="110"/>
-      <c r="CF3" s="110"/>
-      <c r="CG3" s="110"/>
-      <c r="CH3" s="110"/>
-      <c r="CI3" s="110"/>
-      <c r="CJ3" s="110"/>
-      <c r="CK3" s="110"/>
-      <c r="CL3" s="110"/>
-      <c r="CM3" s="110"/>
-      <c r="CN3" s="110"/>
-      <c r="CO3" s="110"/>
-      <c r="CP3" s="110"/>
-      <c r="CQ3" s="110"/>
-      <c r="CR3" s="110"/>
-      <c r="CS3" s="110"/>
-      <c r="CT3" s="110"/>
-      <c r="CU3" s="110"/>
-      <c r="CV3" s="110"/>
-      <c r="CW3" s="110"/>
-      <c r="CX3" s="110"/>
-      <c r="CY3" s="110"/>
-      <c r="CZ3" s="110"/>
-      <c r="DA3" s="110"/>
-      <c r="DB3" s="110"/>
-      <c r="DC3" s="110"/>
-      <c r="DD3" s="110"/>
-      <c r="DE3" s="110"/>
-      <c r="DF3" s="110"/>
-      <c r="DG3" s="110"/>
-      <c r="DH3" s="111"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="108"/>
+      <c r="V3" s="108"/>
+      <c r="W3" s="108"/>
+      <c r="X3" s="108"/>
+      <c r="Y3" s="108"/>
+      <c r="Z3" s="108"/>
+      <c r="AA3" s="108"/>
+      <c r="AB3" s="108"/>
+      <c r="AC3" s="108"/>
+      <c r="AD3" s="108"/>
+      <c r="AE3" s="108"/>
+      <c r="AF3" s="108"/>
+      <c r="AG3" s="108"/>
+      <c r="AH3" s="108"/>
+      <c r="AI3" s="108"/>
+      <c r="AJ3" s="108"/>
+      <c r="AK3" s="108"/>
+      <c r="AL3" s="108"/>
+      <c r="AM3" s="108"/>
+      <c r="AN3" s="108"/>
+      <c r="AO3" s="108"/>
+      <c r="AP3" s="108"/>
+      <c r="AQ3" s="108"/>
+      <c r="AR3" s="108"/>
+      <c r="AS3" s="108"/>
+      <c r="AT3" s="108"/>
+      <c r="AU3" s="108"/>
+      <c r="AV3" s="108"/>
+      <c r="AW3" s="108"/>
+      <c r="AX3" s="108"/>
+      <c r="AY3" s="108"/>
+      <c r="AZ3" s="108"/>
+      <c r="BA3" s="108"/>
+      <c r="BB3" s="108"/>
+      <c r="BC3" s="108"/>
+      <c r="BD3" s="108"/>
+      <c r="BE3" s="108"/>
+      <c r="BF3" s="108"/>
+      <c r="BG3" s="108"/>
+      <c r="BH3" s="108"/>
+      <c r="BI3" s="108"/>
+      <c r="BJ3" s="108"/>
+      <c r="BK3" s="108"/>
+      <c r="BL3" s="108"/>
+      <c r="BM3" s="108"/>
+      <c r="BN3" s="108"/>
+      <c r="BO3" s="108"/>
+      <c r="BP3" s="108"/>
+      <c r="BQ3" s="108"/>
+      <c r="BR3" s="108"/>
+      <c r="BS3" s="108"/>
+      <c r="BT3" s="108"/>
+      <c r="BU3" s="108"/>
+      <c r="BV3" s="108"/>
+      <c r="BW3" s="108"/>
+      <c r="BX3" s="108"/>
+      <c r="BY3" s="108"/>
+      <c r="BZ3" s="108"/>
+      <c r="CA3" s="108"/>
+      <c r="CB3" s="108"/>
+      <c r="CC3" s="108"/>
+      <c r="CD3" s="108"/>
+      <c r="CE3" s="108"/>
+      <c r="CF3" s="108"/>
+      <c r="CG3" s="108"/>
+      <c r="CH3" s="108"/>
+      <c r="CI3" s="108"/>
+      <c r="CJ3" s="108"/>
+      <c r="CK3" s="108"/>
+      <c r="CL3" s="108"/>
+      <c r="CM3" s="108"/>
+      <c r="CN3" s="108"/>
+      <c r="CO3" s="108"/>
+      <c r="CP3" s="108"/>
+      <c r="CQ3" s="108"/>
+      <c r="CR3" s="108"/>
+      <c r="CS3" s="108"/>
+      <c r="CT3" s="108"/>
+      <c r="CU3" s="108"/>
+      <c r="CV3" s="108"/>
+      <c r="CW3" s="108"/>
+      <c r="CX3" s="108"/>
+      <c r="CY3" s="108"/>
+      <c r="CZ3" s="108"/>
+      <c r="DA3" s="108"/>
+      <c r="DB3" s="108"/>
+      <c r="DC3" s="108"/>
+      <c r="DD3" s="108"/>
+      <c r="DE3" s="108"/>
+      <c r="DF3" s="108"/>
+      <c r="DG3" s="108"/>
+      <c r="DH3" s="109"/>
     </row>
     <row r="4" spans="1:112" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="100" t="s">
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="101"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="100" t="s">
+      <c r="H4" s="99"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="102"/>
+      <c r="K4" s="100"/>
       <c r="L4" s="63" t="s">
         <v>16</v>
       </c>
@@ -2131,16 +2145,16 @@
       <c r="DH4" s="28"/>
     </row>
     <row r="5" spans="1:112" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="94"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="105"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="93"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="101"/>
+      <c r="H5" s="102"/>
+      <c r="I5" s="103"/>
+      <c r="J5" s="101"/>
+      <c r="K5" s="103"/>
       <c r="L5" s="64" t="s">
         <v>15</v>
       </c>
@@ -2246,16 +2260,16 @@
       <c r="DH5" s="28"/>
     </row>
     <row r="6" spans="1:112" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="97"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="108"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="106"/>
       <c r="L6" s="51" t="s">
         <v>26</v>
       </c>
@@ -2506,107 +2520,107 @@
       <c r="I8" s="44"/>
       <c r="J8" s="45"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="73"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
-      <c r="S8" s="76"/>
-      <c r="T8" s="76"/>
-      <c r="U8" s="76"/>
-      <c r="V8" s="76"/>
-      <c r="W8" s="76"/>
-      <c r="X8" s="76"/>
-      <c r="Y8" s="76"/>
-      <c r="Z8" s="76"/>
-      <c r="AA8" s="76"/>
-      <c r="AB8" s="76"/>
-      <c r="AC8" s="76"/>
-      <c r="AD8" s="76"/>
-      <c r="AE8" s="76"/>
-      <c r="AF8" s="76"/>
-      <c r="AG8" s="76"/>
-      <c r="AH8" s="76"/>
-      <c r="AI8" s="76"/>
-      <c r="AJ8" s="76"/>
-      <c r="AK8" s="76"/>
-      <c r="AL8" s="76"/>
-      <c r="AM8" s="76"/>
-      <c r="AN8" s="76"/>
-      <c r="AO8" s="76"/>
-      <c r="AP8" s="76"/>
-      <c r="AQ8" s="76"/>
-      <c r="AR8" s="76"/>
-      <c r="AS8" s="76"/>
-      <c r="AT8" s="76"/>
-      <c r="AU8" s="76"/>
-      <c r="AV8" s="76"/>
-      <c r="AW8" s="76"/>
-      <c r="AX8" s="76"/>
-      <c r="AY8" s="76"/>
-      <c r="AZ8" s="76"/>
-      <c r="BA8" s="76"/>
-      <c r="BB8" s="76"/>
-      <c r="BC8" s="76"/>
-      <c r="BD8" s="76"/>
-      <c r="BE8" s="76"/>
-      <c r="BF8" s="76"/>
-      <c r="BG8" s="76"/>
-      <c r="BH8" s="76"/>
-      <c r="BI8" s="76"/>
-      <c r="BJ8" s="76"/>
-      <c r="BK8" s="76"/>
-      <c r="BL8" s="76"/>
-      <c r="BM8" s="76"/>
-      <c r="BN8" s="76"/>
-      <c r="BO8" s="76"/>
-      <c r="BP8" s="76"/>
-      <c r="BQ8" s="76"/>
-      <c r="BR8" s="76"/>
-      <c r="BS8" s="76"/>
-      <c r="BT8" s="76"/>
-      <c r="BU8" s="76"/>
-      <c r="BV8" s="76"/>
-      <c r="BW8" s="76"/>
-      <c r="BX8" s="76"/>
-      <c r="BY8" s="76"/>
-      <c r="BZ8" s="76"/>
-      <c r="CA8" s="76"/>
-      <c r="CB8" s="76"/>
-      <c r="CC8" s="76"/>
-      <c r="CD8" s="76"/>
-      <c r="CE8" s="76"/>
-      <c r="CF8" s="76"/>
-      <c r="CG8" s="76"/>
-      <c r="CH8" s="76"/>
-      <c r="CI8" s="76"/>
-      <c r="CJ8" s="76"/>
-      <c r="CK8" s="76"/>
-      <c r="CL8" s="76"/>
-      <c r="CM8" s="76"/>
-      <c r="CN8" s="76"/>
-      <c r="CO8" s="76"/>
-      <c r="CP8" s="76"/>
-      <c r="CQ8" s="76"/>
-      <c r="CR8" s="76"/>
-      <c r="CS8" s="76"/>
-      <c r="CT8" s="76"/>
-      <c r="CU8" s="76"/>
-      <c r="CV8" s="76"/>
-      <c r="CW8" s="76"/>
-      <c r="CX8" s="76"/>
-      <c r="CY8" s="76"/>
-      <c r="CZ8" s="76"/>
-      <c r="DA8" s="76"/>
-      <c r="DB8" s="76"/>
-      <c r="DC8" s="76"/>
-      <c r="DD8" s="76"/>
-      <c r="DE8" s="76"/>
-      <c r="DF8" s="76"/>
-      <c r="DG8" s="76"/>
-      <c r="DH8" s="77"/>
+      <c r="L8" s="112"/>
+      <c r="M8" s="73"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="74"/>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="74"/>
+      <c r="AG8" s="74"/>
+      <c r="AH8" s="74"/>
+      <c r="AI8" s="74"/>
+      <c r="AJ8" s="74"/>
+      <c r="AK8" s="74"/>
+      <c r="AL8" s="74"/>
+      <c r="AM8" s="74"/>
+      <c r="AN8" s="74"/>
+      <c r="AO8" s="74"/>
+      <c r="AP8" s="74"/>
+      <c r="AQ8" s="74"/>
+      <c r="AR8" s="74"/>
+      <c r="AS8" s="74"/>
+      <c r="AT8" s="74"/>
+      <c r="AU8" s="74"/>
+      <c r="AV8" s="74"/>
+      <c r="AW8" s="74"/>
+      <c r="AX8" s="74"/>
+      <c r="AY8" s="74"/>
+      <c r="AZ8" s="74"/>
+      <c r="BA8" s="74"/>
+      <c r="BB8" s="74"/>
+      <c r="BC8" s="74"/>
+      <c r="BD8" s="74"/>
+      <c r="BE8" s="74"/>
+      <c r="BF8" s="74"/>
+      <c r="BG8" s="74"/>
+      <c r="BH8" s="74"/>
+      <c r="BI8" s="74"/>
+      <c r="BJ8" s="74"/>
+      <c r="BK8" s="74"/>
+      <c r="BL8" s="74"/>
+      <c r="BM8" s="74"/>
+      <c r="BN8" s="74"/>
+      <c r="BO8" s="74"/>
+      <c r="BP8" s="74"/>
+      <c r="BQ8" s="74"/>
+      <c r="BR8" s="74"/>
+      <c r="BS8" s="74"/>
+      <c r="BT8" s="74"/>
+      <c r="BU8" s="74"/>
+      <c r="BV8" s="74"/>
+      <c r="BW8" s="74"/>
+      <c r="BX8" s="74"/>
+      <c r="BY8" s="74"/>
+      <c r="BZ8" s="74"/>
+      <c r="CA8" s="74"/>
+      <c r="CB8" s="74"/>
+      <c r="CC8" s="74"/>
+      <c r="CD8" s="74"/>
+      <c r="CE8" s="74"/>
+      <c r="CF8" s="74"/>
+      <c r="CG8" s="74"/>
+      <c r="CH8" s="74"/>
+      <c r="CI8" s="74"/>
+      <c r="CJ8" s="74"/>
+      <c r="CK8" s="74"/>
+      <c r="CL8" s="74"/>
+      <c r="CM8" s="74"/>
+      <c r="CN8" s="74"/>
+      <c r="CO8" s="74"/>
+      <c r="CP8" s="74"/>
+      <c r="CQ8" s="74"/>
+      <c r="CR8" s="74"/>
+      <c r="CS8" s="74"/>
+      <c r="CT8" s="74"/>
+      <c r="CU8" s="74"/>
+      <c r="CV8" s="74"/>
+      <c r="CW8" s="74"/>
+      <c r="CX8" s="74"/>
+      <c r="CY8" s="74"/>
+      <c r="CZ8" s="74"/>
+      <c r="DA8" s="74"/>
+      <c r="DB8" s="74"/>
+      <c r="DC8" s="74"/>
+      <c r="DD8" s="74"/>
+      <c r="DE8" s="74"/>
+      <c r="DF8" s="74"/>
+      <c r="DG8" s="74"/>
+      <c r="DH8" s="75"/>
     </row>
     <row r="9" spans="1:112" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
@@ -3299,7 +3313,7 @@
       <c r="DH1048575" s="47"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="HwLt1LosB2xo4L1A8DWLPfKLwOWsaMw8F2BWjdF7WR5ENThqXmBOSY+iYaf4qcQmo+PvuV104u2x+l7affR+Kg==" saltValue="9kCQwfl7KbxiAEZxeD/eFQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="j0NcjX851y4PtVYbj98JVHZcIL0PetLE4dhGwBaUCSDiCl+UeH0eLW/8sJLso5EcCoerD4+55D7C3sHDpH2Tog==" saltValue="fbiOfWctC0fVsFWxS5e+Sw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="B4:F6"/>
     <mergeCell ref="G4:I6"/>
@@ -3308,6 +3322,16 @@
     <mergeCell ref="B2:K3"/>
     <mergeCell ref="L2:L3"/>
   </mergeCells>
+  <conditionalFormatting sqref="B8:K1048576">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>B8=""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M8:DH1048576">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>M8=""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L7 C7:J7" xr:uid="{4028DFA7-3B9E-4D78-9BE4-B9C30D52F4E5}">
       <formula1>"&lt;0&gt;0"</formula1>

</xml_diff>

<commit_message>
Form 1-DI extended to 200 data cols
</commit_message>
<xml_diff>
--- a/forms/Form-1DI.xlsx
+++ b/forms/Form-1DI.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283B22F3-39A2-4F16-AB24-05A96F5ECBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C52E6CE-4789-463C-8AB3-F372674CFA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -144,7 +144,32 @@
     <t>Target species</t>
   </si>
   <si>
-    <t>Discards by species, condition, raising, and unit</t>
+    <r>
+      <t xml:space="preserve">Discards by species, condition, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>raising</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and unit</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1015,6 +1040,12 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1116,12 +1147,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1471,24 +1496,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="85"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="87"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="88"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="90"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -1538,15 +1563,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="82"/>
+      <c r="D8" s="84"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="82" t="s">
+      <c r="F8" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="82"/>
+      <c r="G8" s="84"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1717,11 +1742,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="82"/>
+      <c r="G25" s="83"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1761,7 +1786,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:DH1048575"/>
+  <dimension ref="A1:HD1048575"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <pane xSplit="12" ySplit="7" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
@@ -1782,30 +1807,30 @@
     <col min="9" max="9" width="11.42578125" style="69" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="66" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" style="72" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="113" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="80" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="76"/>
-    <col min="14" max="111" width="9.140625" style="77"/>
-    <col min="112" max="112" width="9.140625" style="78"/>
-    <col min="113" max="16384" width="9.140625" style="25"/>
+    <col min="14" max="211" width="9.140625" style="77"/>
+    <col min="212" max="212" width="9.140625" style="78"/>
+    <col min="213" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:212" customFormat="1" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K1" s="38"/>
     </row>
-    <row r="2" spans="1:112" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="83" t="s">
+    <row r="2" spans="1:212" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="110"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="112"/>
       <c r="M2" s="35"/>
       <c r="N2" s="35"/>
       <c r="O2" s="35"/>
@@ -1905,141 +1930,341 @@
       <c r="DE2" s="35"/>
       <c r="DF2" s="35"/>
       <c r="DG2" s="35"/>
-      <c r="DH2" s="36"/>
-    </row>
-    <row r="3" spans="1:112" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DH2" s="35"/>
+      <c r="DI2" s="35"/>
+      <c r="DJ2" s="35"/>
+      <c r="DK2" s="35"/>
+      <c r="DL2" s="35"/>
+      <c r="DM2" s="35"/>
+      <c r="DN2" s="35"/>
+      <c r="DO2" s="35"/>
+      <c r="DP2" s="35"/>
+      <c r="DQ2" s="35"/>
+      <c r="DR2" s="35"/>
+      <c r="DS2" s="35"/>
+      <c r="DT2" s="35"/>
+      <c r="DU2" s="35"/>
+      <c r="DV2" s="35"/>
+      <c r="DW2" s="35"/>
+      <c r="DX2" s="35"/>
+      <c r="DY2" s="35"/>
+      <c r="DZ2" s="35"/>
+      <c r="EA2" s="35"/>
+      <c r="EB2" s="35"/>
+      <c r="EC2" s="35"/>
+      <c r="ED2" s="35"/>
+      <c r="EE2" s="35"/>
+      <c r="EF2" s="35"/>
+      <c r="EG2" s="35"/>
+      <c r="EH2" s="35"/>
+      <c r="EI2" s="35"/>
+      <c r="EJ2" s="35"/>
+      <c r="EK2" s="35"/>
+      <c r="EL2" s="35"/>
+      <c r="EM2" s="35"/>
+      <c r="EN2" s="35"/>
+      <c r="EO2" s="35"/>
+      <c r="EP2" s="35"/>
+      <c r="EQ2" s="35"/>
+      <c r="ER2" s="35"/>
+      <c r="ES2" s="35"/>
+      <c r="ET2" s="35"/>
+      <c r="EU2" s="35"/>
+      <c r="EV2" s="35"/>
+      <c r="EW2" s="35"/>
+      <c r="EX2" s="35"/>
+      <c r="EY2" s="35"/>
+      <c r="EZ2" s="35"/>
+      <c r="FA2" s="35"/>
+      <c r="FB2" s="35"/>
+      <c r="FC2" s="35"/>
+      <c r="FD2" s="35"/>
+      <c r="FE2" s="35"/>
+      <c r="FF2" s="35"/>
+      <c r="FG2" s="35"/>
+      <c r="FH2" s="35"/>
+      <c r="FI2" s="35"/>
+      <c r="FJ2" s="35"/>
+      <c r="FK2" s="35"/>
+      <c r="FL2" s="35"/>
+      <c r="FM2" s="35"/>
+      <c r="FN2" s="35"/>
+      <c r="FO2" s="35"/>
+      <c r="FP2" s="35"/>
+      <c r="FQ2" s="35"/>
+      <c r="FR2" s="35"/>
+      <c r="FS2" s="35"/>
+      <c r="FT2" s="35"/>
+      <c r="FU2" s="35"/>
+      <c r="FV2" s="35"/>
+      <c r="FW2" s="35"/>
+      <c r="FX2" s="35"/>
+      <c r="FY2" s="35"/>
+      <c r="FZ2" s="35"/>
+      <c r="GA2" s="35"/>
+      <c r="GB2" s="35"/>
+      <c r="GC2" s="35"/>
+      <c r="GD2" s="35"/>
+      <c r="GE2" s="35"/>
+      <c r="GF2" s="35"/>
+      <c r="GG2" s="35"/>
+      <c r="GH2" s="35"/>
+      <c r="GI2" s="35"/>
+      <c r="GJ2" s="35"/>
+      <c r="GK2" s="35"/>
+      <c r="GL2" s="35"/>
+      <c r="GM2" s="35"/>
+      <c r="GN2" s="35"/>
+      <c r="GO2" s="35"/>
+      <c r="GP2" s="35"/>
+      <c r="GQ2" s="35"/>
+      <c r="GR2" s="35"/>
+      <c r="GS2" s="35"/>
+      <c r="GT2" s="35"/>
+      <c r="GU2" s="35"/>
+      <c r="GV2" s="35"/>
+      <c r="GW2" s="35"/>
+      <c r="GX2" s="35"/>
+      <c r="GY2" s="35"/>
+      <c r="GZ2" s="35"/>
+      <c r="HA2" s="35"/>
+      <c r="HB2" s="35"/>
+      <c r="HC2" s="35"/>
+      <c r="HD2" s="36"/>
+    </row>
+    <row r="3" spans="1:212" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="111"/>
-      <c r="M3" s="107" t="s">
+      <c r="B3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="113"/>
+      <c r="M3" s="109" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="108"/>
-      <c r="X3" s="108"/>
-      <c r="Y3" s="108"/>
-      <c r="Z3" s="108"/>
-      <c r="AA3" s="108"/>
-      <c r="AB3" s="108"/>
-      <c r="AC3" s="108"/>
-      <c r="AD3" s="108"/>
-      <c r="AE3" s="108"/>
-      <c r="AF3" s="108"/>
-      <c r="AG3" s="108"/>
-      <c r="AH3" s="108"/>
-      <c r="AI3" s="108"/>
-      <c r="AJ3" s="108"/>
-      <c r="AK3" s="108"/>
-      <c r="AL3" s="108"/>
-      <c r="AM3" s="108"/>
-      <c r="AN3" s="108"/>
-      <c r="AO3" s="108"/>
-      <c r="AP3" s="108"/>
-      <c r="AQ3" s="108"/>
-      <c r="AR3" s="108"/>
-      <c r="AS3" s="108"/>
-      <c r="AT3" s="108"/>
-      <c r="AU3" s="108"/>
-      <c r="AV3" s="108"/>
-      <c r="AW3" s="108"/>
-      <c r="AX3" s="108"/>
-      <c r="AY3" s="108"/>
-      <c r="AZ3" s="108"/>
-      <c r="BA3" s="108"/>
-      <c r="BB3" s="108"/>
-      <c r="BC3" s="108"/>
-      <c r="BD3" s="108"/>
-      <c r="BE3" s="108"/>
-      <c r="BF3" s="108"/>
-      <c r="BG3" s="108"/>
-      <c r="BH3" s="108"/>
-      <c r="BI3" s="108"/>
-      <c r="BJ3" s="108"/>
-      <c r="BK3" s="108"/>
-      <c r="BL3" s="108"/>
-      <c r="BM3" s="108"/>
-      <c r="BN3" s="108"/>
-      <c r="BO3" s="108"/>
-      <c r="BP3" s="108"/>
-      <c r="BQ3" s="108"/>
-      <c r="BR3" s="108"/>
-      <c r="BS3" s="108"/>
-      <c r="BT3" s="108"/>
-      <c r="BU3" s="108"/>
-      <c r="BV3" s="108"/>
-      <c r="BW3" s="108"/>
-      <c r="BX3" s="108"/>
-      <c r="BY3" s="108"/>
-      <c r="BZ3" s="108"/>
-      <c r="CA3" s="108"/>
-      <c r="CB3" s="108"/>
-      <c r="CC3" s="108"/>
-      <c r="CD3" s="108"/>
-      <c r="CE3" s="108"/>
-      <c r="CF3" s="108"/>
-      <c r="CG3" s="108"/>
-      <c r="CH3" s="108"/>
-      <c r="CI3" s="108"/>
-      <c r="CJ3" s="108"/>
-      <c r="CK3" s="108"/>
-      <c r="CL3" s="108"/>
-      <c r="CM3" s="108"/>
-      <c r="CN3" s="108"/>
-      <c r="CO3" s="108"/>
-      <c r="CP3" s="108"/>
-      <c r="CQ3" s="108"/>
-      <c r="CR3" s="108"/>
-      <c r="CS3" s="108"/>
-      <c r="CT3" s="108"/>
-      <c r="CU3" s="108"/>
-      <c r="CV3" s="108"/>
-      <c r="CW3" s="108"/>
-      <c r="CX3" s="108"/>
-      <c r="CY3" s="108"/>
-      <c r="CZ3" s="108"/>
-      <c r="DA3" s="108"/>
-      <c r="DB3" s="108"/>
-      <c r="DC3" s="108"/>
-      <c r="DD3" s="108"/>
-      <c r="DE3" s="108"/>
-      <c r="DF3" s="108"/>
-      <c r="DG3" s="108"/>
-      <c r="DH3" s="109"/>
-    </row>
-    <row r="4" spans="1:112" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="89" t="s">
+      <c r="N3" s="110"/>
+      <c r="O3" s="110"/>
+      <c r="P3" s="110"/>
+      <c r="Q3" s="110"/>
+      <c r="R3" s="110"/>
+      <c r="S3" s="110"/>
+      <c r="T3" s="110"/>
+      <c r="U3" s="110"/>
+      <c r="V3" s="110"/>
+      <c r="W3" s="110"/>
+      <c r="X3" s="110"/>
+      <c r="Y3" s="110"/>
+      <c r="Z3" s="110"/>
+      <c r="AA3" s="110"/>
+      <c r="AB3" s="110"/>
+      <c r="AC3" s="110"/>
+      <c r="AD3" s="110"/>
+      <c r="AE3" s="110"/>
+      <c r="AF3" s="110"/>
+      <c r="AG3" s="110"/>
+      <c r="AH3" s="110"/>
+      <c r="AI3" s="110"/>
+      <c r="AJ3" s="110"/>
+      <c r="AK3" s="110"/>
+      <c r="AL3" s="110"/>
+      <c r="AM3" s="110"/>
+      <c r="AN3" s="110"/>
+      <c r="AO3" s="110"/>
+      <c r="AP3" s="110"/>
+      <c r="AQ3" s="110"/>
+      <c r="AR3" s="110"/>
+      <c r="AS3" s="110"/>
+      <c r="AT3" s="110"/>
+      <c r="AU3" s="110"/>
+      <c r="AV3" s="110"/>
+      <c r="AW3" s="110"/>
+      <c r="AX3" s="110"/>
+      <c r="AY3" s="110"/>
+      <c r="AZ3" s="110"/>
+      <c r="BA3" s="110"/>
+      <c r="BB3" s="110"/>
+      <c r="BC3" s="110"/>
+      <c r="BD3" s="110"/>
+      <c r="BE3" s="110"/>
+      <c r="BF3" s="110"/>
+      <c r="BG3" s="110"/>
+      <c r="BH3" s="110"/>
+      <c r="BI3" s="110"/>
+      <c r="BJ3" s="110"/>
+      <c r="BK3" s="110"/>
+      <c r="BL3" s="110"/>
+      <c r="BM3" s="110"/>
+      <c r="BN3" s="110"/>
+      <c r="BO3" s="110"/>
+      <c r="BP3" s="110"/>
+      <c r="BQ3" s="110"/>
+      <c r="BR3" s="110"/>
+      <c r="BS3" s="110"/>
+      <c r="BT3" s="110"/>
+      <c r="BU3" s="110"/>
+      <c r="BV3" s="110"/>
+      <c r="BW3" s="110"/>
+      <c r="BX3" s="110"/>
+      <c r="BY3" s="110"/>
+      <c r="BZ3" s="110"/>
+      <c r="CA3" s="110"/>
+      <c r="CB3" s="110"/>
+      <c r="CC3" s="110"/>
+      <c r="CD3" s="110"/>
+      <c r="CE3" s="110"/>
+      <c r="CF3" s="110"/>
+      <c r="CG3" s="110"/>
+      <c r="CH3" s="110"/>
+      <c r="CI3" s="110"/>
+      <c r="CJ3" s="110"/>
+      <c r="CK3" s="110"/>
+      <c r="CL3" s="110"/>
+      <c r="CM3" s="110"/>
+      <c r="CN3" s="110"/>
+      <c r="CO3" s="110"/>
+      <c r="CP3" s="110"/>
+      <c r="CQ3" s="110"/>
+      <c r="CR3" s="110"/>
+      <c r="CS3" s="110"/>
+      <c r="CT3" s="110"/>
+      <c r="CU3" s="110"/>
+      <c r="CV3" s="110"/>
+      <c r="CW3" s="110"/>
+      <c r="CX3" s="110"/>
+      <c r="CY3" s="110"/>
+      <c r="CZ3" s="110"/>
+      <c r="DA3" s="110"/>
+      <c r="DB3" s="110"/>
+      <c r="DC3" s="110"/>
+      <c r="DD3" s="110"/>
+      <c r="DE3" s="110"/>
+      <c r="DF3" s="110"/>
+      <c r="DG3" s="110"/>
+      <c r="DH3" s="110"/>
+      <c r="DI3" s="110"/>
+      <c r="DJ3" s="110"/>
+      <c r="DK3" s="110"/>
+      <c r="DL3" s="110"/>
+      <c r="DM3" s="110"/>
+      <c r="DN3" s="110"/>
+      <c r="DO3" s="110"/>
+      <c r="DP3" s="110"/>
+      <c r="DQ3" s="110"/>
+      <c r="DR3" s="110"/>
+      <c r="DS3" s="110"/>
+      <c r="DT3" s="110"/>
+      <c r="DU3" s="110"/>
+      <c r="DV3" s="110"/>
+      <c r="DW3" s="110"/>
+      <c r="DX3" s="110"/>
+      <c r="DY3" s="110"/>
+      <c r="DZ3" s="110"/>
+      <c r="EA3" s="110"/>
+      <c r="EB3" s="110"/>
+      <c r="EC3" s="110"/>
+      <c r="ED3" s="110"/>
+      <c r="EE3" s="110"/>
+      <c r="EF3" s="110"/>
+      <c r="EG3" s="110"/>
+      <c r="EH3" s="110"/>
+      <c r="EI3" s="110"/>
+      <c r="EJ3" s="110"/>
+      <c r="EK3" s="110"/>
+      <c r="EL3" s="110"/>
+      <c r="EM3" s="110"/>
+      <c r="EN3" s="110"/>
+      <c r="EO3" s="110"/>
+      <c r="EP3" s="110"/>
+      <c r="EQ3" s="110"/>
+      <c r="ER3" s="110"/>
+      <c r="ES3" s="110"/>
+      <c r="ET3" s="110"/>
+      <c r="EU3" s="110"/>
+      <c r="EV3" s="110"/>
+      <c r="EW3" s="110"/>
+      <c r="EX3" s="110"/>
+      <c r="EY3" s="110"/>
+      <c r="EZ3" s="110"/>
+      <c r="FA3" s="110"/>
+      <c r="FB3" s="110"/>
+      <c r="FC3" s="110"/>
+      <c r="FD3" s="110"/>
+      <c r="FE3" s="110"/>
+      <c r="FF3" s="110"/>
+      <c r="FG3" s="110"/>
+      <c r="FH3" s="110"/>
+      <c r="FI3" s="110"/>
+      <c r="FJ3" s="110"/>
+      <c r="FK3" s="110"/>
+      <c r="FL3" s="110"/>
+      <c r="FM3" s="110"/>
+      <c r="FN3" s="110"/>
+      <c r="FO3" s="110"/>
+      <c r="FP3" s="110"/>
+      <c r="FQ3" s="110"/>
+      <c r="FR3" s="110"/>
+      <c r="FS3" s="110"/>
+      <c r="FT3" s="110"/>
+      <c r="FU3" s="110"/>
+      <c r="FV3" s="110"/>
+      <c r="FW3" s="110"/>
+      <c r="FX3" s="110"/>
+      <c r="FY3" s="110"/>
+      <c r="FZ3" s="110"/>
+      <c r="GA3" s="110"/>
+      <c r="GB3" s="110"/>
+      <c r="GC3" s="110"/>
+      <c r="GD3" s="110"/>
+      <c r="GE3" s="110"/>
+      <c r="GF3" s="110"/>
+      <c r="GG3" s="110"/>
+      <c r="GH3" s="110"/>
+      <c r="GI3" s="110"/>
+      <c r="GJ3" s="110"/>
+      <c r="GK3" s="110"/>
+      <c r="GL3" s="110"/>
+      <c r="GM3" s="110"/>
+      <c r="GN3" s="110"/>
+      <c r="GO3" s="110"/>
+      <c r="GP3" s="110"/>
+      <c r="GQ3" s="110"/>
+      <c r="GR3" s="110"/>
+      <c r="GS3" s="110"/>
+      <c r="GT3" s="110"/>
+      <c r="GU3" s="110"/>
+      <c r="GV3" s="110"/>
+      <c r="GW3" s="110"/>
+      <c r="GX3" s="110"/>
+      <c r="GY3" s="110"/>
+      <c r="GZ3" s="110"/>
+      <c r="HA3" s="110"/>
+      <c r="HB3" s="110"/>
+      <c r="HC3" s="110"/>
+      <c r="HD3" s="111"/>
+    </row>
+    <row r="4" spans="1:212" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="98" t="s">
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="99"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="98" t="s">
+      <c r="H4" s="101"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="100"/>
+      <c r="K4" s="102"/>
       <c r="L4" s="63" t="s">
         <v>16</v>
       </c>
@@ -2142,19 +2367,119 @@
       <c r="DE4" s="27"/>
       <c r="DF4" s="27"/>
       <c r="DG4" s="27"/>
-      <c r="DH4" s="28"/>
-    </row>
-    <row r="5" spans="1:112" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="92"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="101"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="103"/>
-      <c r="J5" s="101"/>
-      <c r="K5" s="103"/>
+      <c r="DH4" s="27"/>
+      <c r="DI4" s="27"/>
+      <c r="DJ4" s="27"/>
+      <c r="DK4" s="27"/>
+      <c r="DL4" s="27"/>
+      <c r="DM4" s="27"/>
+      <c r="DN4" s="27"/>
+      <c r="DO4" s="27"/>
+      <c r="DP4" s="27"/>
+      <c r="DQ4" s="27"/>
+      <c r="DR4" s="27"/>
+      <c r="DS4" s="27"/>
+      <c r="DT4" s="27"/>
+      <c r="DU4" s="27"/>
+      <c r="DV4" s="27"/>
+      <c r="DW4" s="27"/>
+      <c r="DX4" s="27"/>
+      <c r="DY4" s="27"/>
+      <c r="DZ4" s="27"/>
+      <c r="EA4" s="27"/>
+      <c r="EB4" s="27"/>
+      <c r="EC4" s="27"/>
+      <c r="ED4" s="27"/>
+      <c r="EE4" s="27"/>
+      <c r="EF4" s="27"/>
+      <c r="EG4" s="27"/>
+      <c r="EH4" s="27"/>
+      <c r="EI4" s="27"/>
+      <c r="EJ4" s="27"/>
+      <c r="EK4" s="27"/>
+      <c r="EL4" s="27"/>
+      <c r="EM4" s="27"/>
+      <c r="EN4" s="27"/>
+      <c r="EO4" s="27"/>
+      <c r="EP4" s="27"/>
+      <c r="EQ4" s="27"/>
+      <c r="ER4" s="27"/>
+      <c r="ES4" s="27"/>
+      <c r="ET4" s="27"/>
+      <c r="EU4" s="27"/>
+      <c r="EV4" s="27"/>
+      <c r="EW4" s="27"/>
+      <c r="EX4" s="27"/>
+      <c r="EY4" s="27"/>
+      <c r="EZ4" s="27"/>
+      <c r="FA4" s="27"/>
+      <c r="FB4" s="27"/>
+      <c r="FC4" s="27"/>
+      <c r="FD4" s="27"/>
+      <c r="FE4" s="27"/>
+      <c r="FF4" s="27"/>
+      <c r="FG4" s="27"/>
+      <c r="FH4" s="27"/>
+      <c r="FI4" s="27"/>
+      <c r="FJ4" s="27"/>
+      <c r="FK4" s="27"/>
+      <c r="FL4" s="27"/>
+      <c r="FM4" s="27"/>
+      <c r="FN4" s="27"/>
+      <c r="FO4" s="27"/>
+      <c r="FP4" s="27"/>
+      <c r="FQ4" s="27"/>
+      <c r="FR4" s="27"/>
+      <c r="FS4" s="27"/>
+      <c r="FT4" s="27"/>
+      <c r="FU4" s="27"/>
+      <c r="FV4" s="27"/>
+      <c r="FW4" s="27"/>
+      <c r="FX4" s="27"/>
+      <c r="FY4" s="27"/>
+      <c r="FZ4" s="27"/>
+      <c r="GA4" s="27"/>
+      <c r="GB4" s="27"/>
+      <c r="GC4" s="27"/>
+      <c r="GD4" s="27"/>
+      <c r="GE4" s="27"/>
+      <c r="GF4" s="27"/>
+      <c r="GG4" s="27"/>
+      <c r="GH4" s="27"/>
+      <c r="GI4" s="27"/>
+      <c r="GJ4" s="27"/>
+      <c r="GK4" s="27"/>
+      <c r="GL4" s="27"/>
+      <c r="GM4" s="27"/>
+      <c r="GN4" s="27"/>
+      <c r="GO4" s="27"/>
+      <c r="GP4" s="27"/>
+      <c r="GQ4" s="27"/>
+      <c r="GR4" s="27"/>
+      <c r="GS4" s="27"/>
+      <c r="GT4" s="27"/>
+      <c r="GU4" s="27"/>
+      <c r="GV4" s="27"/>
+      <c r="GW4" s="27"/>
+      <c r="GX4" s="27"/>
+      <c r="GY4" s="27"/>
+      <c r="GZ4" s="27"/>
+      <c r="HA4" s="27"/>
+      <c r="HB4" s="27"/>
+      <c r="HC4" s="27"/>
+      <c r="HD4" s="28"/>
+    </row>
+    <row r="5" spans="1:212" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="94"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="105"/>
       <c r="L5" s="64" t="s">
         <v>15</v>
       </c>
@@ -2257,19 +2582,119 @@
       <c r="DE5" s="27"/>
       <c r="DF5" s="27"/>
       <c r="DG5" s="27"/>
-      <c r="DH5" s="28"/>
-    </row>
-    <row r="6" spans="1:112" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="95"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="104"/>
-      <c r="H6" s="105"/>
-      <c r="I6" s="106"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="106"/>
+      <c r="DH5" s="27"/>
+      <c r="DI5" s="27"/>
+      <c r="DJ5" s="27"/>
+      <c r="DK5" s="27"/>
+      <c r="DL5" s="27"/>
+      <c r="DM5" s="27"/>
+      <c r="DN5" s="27"/>
+      <c r="DO5" s="27"/>
+      <c r="DP5" s="27"/>
+      <c r="DQ5" s="27"/>
+      <c r="DR5" s="27"/>
+      <c r="DS5" s="27"/>
+      <c r="DT5" s="27"/>
+      <c r="DU5" s="27"/>
+      <c r="DV5" s="27"/>
+      <c r="DW5" s="27"/>
+      <c r="DX5" s="27"/>
+      <c r="DY5" s="27"/>
+      <c r="DZ5" s="27"/>
+      <c r="EA5" s="27"/>
+      <c r="EB5" s="27"/>
+      <c r="EC5" s="27"/>
+      <c r="ED5" s="27"/>
+      <c r="EE5" s="27"/>
+      <c r="EF5" s="27"/>
+      <c r="EG5" s="27"/>
+      <c r="EH5" s="27"/>
+      <c r="EI5" s="27"/>
+      <c r="EJ5" s="27"/>
+      <c r="EK5" s="27"/>
+      <c r="EL5" s="27"/>
+      <c r="EM5" s="27"/>
+      <c r="EN5" s="27"/>
+      <c r="EO5" s="27"/>
+      <c r="EP5" s="27"/>
+      <c r="EQ5" s="27"/>
+      <c r="ER5" s="27"/>
+      <c r="ES5" s="27"/>
+      <c r="ET5" s="27"/>
+      <c r="EU5" s="27"/>
+      <c r="EV5" s="27"/>
+      <c r="EW5" s="27"/>
+      <c r="EX5" s="27"/>
+      <c r="EY5" s="27"/>
+      <c r="EZ5" s="27"/>
+      <c r="FA5" s="27"/>
+      <c r="FB5" s="27"/>
+      <c r="FC5" s="27"/>
+      <c r="FD5" s="27"/>
+      <c r="FE5" s="27"/>
+      <c r="FF5" s="27"/>
+      <c r="FG5" s="27"/>
+      <c r="FH5" s="27"/>
+      <c r="FI5" s="27"/>
+      <c r="FJ5" s="27"/>
+      <c r="FK5" s="27"/>
+      <c r="FL5" s="27"/>
+      <c r="FM5" s="27"/>
+      <c r="FN5" s="27"/>
+      <c r="FO5" s="27"/>
+      <c r="FP5" s="27"/>
+      <c r="FQ5" s="27"/>
+      <c r="FR5" s="27"/>
+      <c r="FS5" s="27"/>
+      <c r="FT5" s="27"/>
+      <c r="FU5" s="27"/>
+      <c r="FV5" s="27"/>
+      <c r="FW5" s="27"/>
+      <c r="FX5" s="27"/>
+      <c r="FY5" s="27"/>
+      <c r="FZ5" s="27"/>
+      <c r="GA5" s="27"/>
+      <c r="GB5" s="27"/>
+      <c r="GC5" s="27"/>
+      <c r="GD5" s="27"/>
+      <c r="GE5" s="27"/>
+      <c r="GF5" s="27"/>
+      <c r="GG5" s="27"/>
+      <c r="GH5" s="27"/>
+      <c r="GI5" s="27"/>
+      <c r="GJ5" s="27"/>
+      <c r="GK5" s="27"/>
+      <c r="GL5" s="27"/>
+      <c r="GM5" s="27"/>
+      <c r="GN5" s="27"/>
+      <c r="GO5" s="27"/>
+      <c r="GP5" s="27"/>
+      <c r="GQ5" s="27"/>
+      <c r="GR5" s="27"/>
+      <c r="GS5" s="27"/>
+      <c r="GT5" s="27"/>
+      <c r="GU5" s="27"/>
+      <c r="GV5" s="27"/>
+      <c r="GW5" s="27"/>
+      <c r="GX5" s="27"/>
+      <c r="GY5" s="27"/>
+      <c r="GZ5" s="27"/>
+      <c r="HA5" s="27"/>
+      <c r="HB5" s="27"/>
+      <c r="HC5" s="27"/>
+      <c r="HD5" s="28"/>
+    </row>
+    <row r="6" spans="1:212" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="97"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="108"/>
       <c r="L6" s="51" t="s">
         <v>26</v>
       </c>
@@ -2372,9 +2797,109 @@
       <c r="DE6" s="27"/>
       <c r="DF6" s="27"/>
       <c r="DG6" s="27"/>
-      <c r="DH6" s="28"/>
-    </row>
-    <row r="7" spans="1:112" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DH6" s="27"/>
+      <c r="DI6" s="27"/>
+      <c r="DJ6" s="27"/>
+      <c r="DK6" s="27"/>
+      <c r="DL6" s="27"/>
+      <c r="DM6" s="27"/>
+      <c r="DN6" s="27"/>
+      <c r="DO6" s="27"/>
+      <c r="DP6" s="27"/>
+      <c r="DQ6" s="27"/>
+      <c r="DR6" s="27"/>
+      <c r="DS6" s="27"/>
+      <c r="DT6" s="27"/>
+      <c r="DU6" s="27"/>
+      <c r="DV6" s="27"/>
+      <c r="DW6" s="27"/>
+      <c r="DX6" s="27"/>
+      <c r="DY6" s="27"/>
+      <c r="DZ6" s="27"/>
+      <c r="EA6" s="27"/>
+      <c r="EB6" s="27"/>
+      <c r="EC6" s="27"/>
+      <c r="ED6" s="27"/>
+      <c r="EE6" s="27"/>
+      <c r="EF6" s="27"/>
+      <c r="EG6" s="27"/>
+      <c r="EH6" s="27"/>
+      <c r="EI6" s="27"/>
+      <c r="EJ6" s="27"/>
+      <c r="EK6" s="27"/>
+      <c r="EL6" s="27"/>
+      <c r="EM6" s="27"/>
+      <c r="EN6" s="27"/>
+      <c r="EO6" s="27"/>
+      <c r="EP6" s="27"/>
+      <c r="EQ6" s="27"/>
+      <c r="ER6" s="27"/>
+      <c r="ES6" s="27"/>
+      <c r="ET6" s="27"/>
+      <c r="EU6" s="27"/>
+      <c r="EV6" s="27"/>
+      <c r="EW6" s="27"/>
+      <c r="EX6" s="27"/>
+      <c r="EY6" s="27"/>
+      <c r="EZ6" s="27"/>
+      <c r="FA6" s="27"/>
+      <c r="FB6" s="27"/>
+      <c r="FC6" s="27"/>
+      <c r="FD6" s="27"/>
+      <c r="FE6" s="27"/>
+      <c r="FF6" s="27"/>
+      <c r="FG6" s="27"/>
+      <c r="FH6" s="27"/>
+      <c r="FI6" s="27"/>
+      <c r="FJ6" s="27"/>
+      <c r="FK6" s="27"/>
+      <c r="FL6" s="27"/>
+      <c r="FM6" s="27"/>
+      <c r="FN6" s="27"/>
+      <c r="FO6" s="27"/>
+      <c r="FP6" s="27"/>
+      <c r="FQ6" s="27"/>
+      <c r="FR6" s="27"/>
+      <c r="FS6" s="27"/>
+      <c r="FT6" s="27"/>
+      <c r="FU6" s="27"/>
+      <c r="FV6" s="27"/>
+      <c r="FW6" s="27"/>
+      <c r="FX6" s="27"/>
+      <c r="FY6" s="27"/>
+      <c r="FZ6" s="27"/>
+      <c r="GA6" s="27"/>
+      <c r="GB6" s="27"/>
+      <c r="GC6" s="27"/>
+      <c r="GD6" s="27"/>
+      <c r="GE6" s="27"/>
+      <c r="GF6" s="27"/>
+      <c r="GG6" s="27"/>
+      <c r="GH6" s="27"/>
+      <c r="GI6" s="27"/>
+      <c r="GJ6" s="27"/>
+      <c r="GK6" s="27"/>
+      <c r="GL6" s="27"/>
+      <c r="GM6" s="27"/>
+      <c r="GN6" s="27"/>
+      <c r="GO6" s="27"/>
+      <c r="GP6" s="27"/>
+      <c r="GQ6" s="27"/>
+      <c r="GR6" s="27"/>
+      <c r="GS6" s="27"/>
+      <c r="GT6" s="27"/>
+      <c r="GU6" s="27"/>
+      <c r="GV6" s="27"/>
+      <c r="GW6" s="27"/>
+      <c r="GX6" s="27"/>
+      <c r="GY6" s="27"/>
+      <c r="GZ6" s="27"/>
+      <c r="HA6" s="27"/>
+      <c r="HB6" s="27"/>
+      <c r="HC6" s="27"/>
+      <c r="HD6" s="28"/>
+    </row>
+    <row r="7" spans="1:212" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="54" t="s">
         <v>14</v>
       </c>
@@ -2507,9 +3032,109 @@
       <c r="DE7" s="30"/>
       <c r="DF7" s="30"/>
       <c r="DG7" s="30"/>
-      <c r="DH7" s="31"/>
-    </row>
-    <row r="8" spans="1:112" x14ac:dyDescent="0.25">
+      <c r="DH7" s="30"/>
+      <c r="DI7" s="30"/>
+      <c r="DJ7" s="30"/>
+      <c r="DK7" s="30"/>
+      <c r="DL7" s="30"/>
+      <c r="DM7" s="30"/>
+      <c r="DN7" s="30"/>
+      <c r="DO7" s="30"/>
+      <c r="DP7" s="30"/>
+      <c r="DQ7" s="30"/>
+      <c r="DR7" s="30"/>
+      <c r="DS7" s="30"/>
+      <c r="DT7" s="30"/>
+      <c r="DU7" s="30"/>
+      <c r="DV7" s="30"/>
+      <c r="DW7" s="30"/>
+      <c r="DX7" s="30"/>
+      <c r="DY7" s="30"/>
+      <c r="DZ7" s="30"/>
+      <c r="EA7" s="30"/>
+      <c r="EB7" s="30"/>
+      <c r="EC7" s="30"/>
+      <c r="ED7" s="30"/>
+      <c r="EE7" s="30"/>
+      <c r="EF7" s="30"/>
+      <c r="EG7" s="30"/>
+      <c r="EH7" s="30"/>
+      <c r="EI7" s="30"/>
+      <c r="EJ7" s="30"/>
+      <c r="EK7" s="30"/>
+      <c r="EL7" s="30"/>
+      <c r="EM7" s="30"/>
+      <c r="EN7" s="30"/>
+      <c r="EO7" s="30"/>
+      <c r="EP7" s="30"/>
+      <c r="EQ7" s="30"/>
+      <c r="ER7" s="30"/>
+      <c r="ES7" s="30"/>
+      <c r="ET7" s="30"/>
+      <c r="EU7" s="30"/>
+      <c r="EV7" s="30"/>
+      <c r="EW7" s="30"/>
+      <c r="EX7" s="30"/>
+      <c r="EY7" s="30"/>
+      <c r="EZ7" s="30"/>
+      <c r="FA7" s="30"/>
+      <c r="FB7" s="30"/>
+      <c r="FC7" s="30"/>
+      <c r="FD7" s="30"/>
+      <c r="FE7" s="30"/>
+      <c r="FF7" s="30"/>
+      <c r="FG7" s="30"/>
+      <c r="FH7" s="30"/>
+      <c r="FI7" s="30"/>
+      <c r="FJ7" s="30"/>
+      <c r="FK7" s="30"/>
+      <c r="FL7" s="30"/>
+      <c r="FM7" s="30"/>
+      <c r="FN7" s="30"/>
+      <c r="FO7" s="30"/>
+      <c r="FP7" s="30"/>
+      <c r="FQ7" s="30"/>
+      <c r="FR7" s="30"/>
+      <c r="FS7" s="30"/>
+      <c r="FT7" s="30"/>
+      <c r="FU7" s="30"/>
+      <c r="FV7" s="30"/>
+      <c r="FW7" s="30"/>
+      <c r="FX7" s="30"/>
+      <c r="FY7" s="30"/>
+      <c r="FZ7" s="30"/>
+      <c r="GA7" s="30"/>
+      <c r="GB7" s="30"/>
+      <c r="GC7" s="30"/>
+      <c r="GD7" s="30"/>
+      <c r="GE7" s="30"/>
+      <c r="GF7" s="30"/>
+      <c r="GG7" s="30"/>
+      <c r="GH7" s="30"/>
+      <c r="GI7" s="30"/>
+      <c r="GJ7" s="30"/>
+      <c r="GK7" s="30"/>
+      <c r="GL7" s="30"/>
+      <c r="GM7" s="30"/>
+      <c r="GN7" s="30"/>
+      <c r="GO7" s="30"/>
+      <c r="GP7" s="30"/>
+      <c r="GQ7" s="30"/>
+      <c r="GR7" s="30"/>
+      <c r="GS7" s="30"/>
+      <c r="GT7" s="30"/>
+      <c r="GU7" s="30"/>
+      <c r="GV7" s="30"/>
+      <c r="GW7" s="30"/>
+      <c r="GX7" s="30"/>
+      <c r="GY7" s="30"/>
+      <c r="GZ7" s="30"/>
+      <c r="HA7" s="30"/>
+      <c r="HB7" s="30"/>
+      <c r="HC7" s="30"/>
+      <c r="HD7" s="31"/>
+    </row>
+    <row r="8" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B8" s="42"/>
       <c r="C8" s="43"/>
       <c r="D8" s="43"/>
@@ -2520,7 +3145,7 @@
       <c r="I8" s="44"/>
       <c r="J8" s="45"/>
       <c r="K8" s="70"/>
-      <c r="L8" s="112"/>
+      <c r="L8" s="79"/>
       <c r="M8" s="73"/>
       <c r="N8" s="74"/>
       <c r="O8" s="74"/>
@@ -2620,9 +3245,109 @@
       <c r="DE8" s="74"/>
       <c r="DF8" s="74"/>
       <c r="DG8" s="74"/>
-      <c r="DH8" s="75"/>
-    </row>
-    <row r="9" spans="1:112" x14ac:dyDescent="0.25">
+      <c r="DH8" s="74"/>
+      <c r="DI8" s="74"/>
+      <c r="DJ8" s="74"/>
+      <c r="DK8" s="74"/>
+      <c r="DL8" s="74"/>
+      <c r="DM8" s="74"/>
+      <c r="DN8" s="74"/>
+      <c r="DO8" s="74"/>
+      <c r="DP8" s="74"/>
+      <c r="DQ8" s="74"/>
+      <c r="DR8" s="74"/>
+      <c r="DS8" s="74"/>
+      <c r="DT8" s="74"/>
+      <c r="DU8" s="74"/>
+      <c r="DV8" s="74"/>
+      <c r="DW8" s="74"/>
+      <c r="DX8" s="74"/>
+      <c r="DY8" s="74"/>
+      <c r="DZ8" s="74"/>
+      <c r="EA8" s="74"/>
+      <c r="EB8" s="74"/>
+      <c r="EC8" s="74"/>
+      <c r="ED8" s="74"/>
+      <c r="EE8" s="74"/>
+      <c r="EF8" s="74"/>
+      <c r="EG8" s="74"/>
+      <c r="EH8" s="74"/>
+      <c r="EI8" s="74"/>
+      <c r="EJ8" s="74"/>
+      <c r="EK8" s="74"/>
+      <c r="EL8" s="74"/>
+      <c r="EM8" s="74"/>
+      <c r="EN8" s="74"/>
+      <c r="EO8" s="74"/>
+      <c r="EP8" s="74"/>
+      <c r="EQ8" s="74"/>
+      <c r="ER8" s="74"/>
+      <c r="ES8" s="74"/>
+      <c r="ET8" s="74"/>
+      <c r="EU8" s="74"/>
+      <c r="EV8" s="74"/>
+      <c r="EW8" s="74"/>
+      <c r="EX8" s="74"/>
+      <c r="EY8" s="74"/>
+      <c r="EZ8" s="74"/>
+      <c r="FA8" s="74"/>
+      <c r="FB8" s="74"/>
+      <c r="FC8" s="74"/>
+      <c r="FD8" s="74"/>
+      <c r="FE8" s="74"/>
+      <c r="FF8" s="74"/>
+      <c r="FG8" s="74"/>
+      <c r="FH8" s="74"/>
+      <c r="FI8" s="74"/>
+      <c r="FJ8" s="74"/>
+      <c r="FK8" s="74"/>
+      <c r="FL8" s="74"/>
+      <c r="FM8" s="74"/>
+      <c r="FN8" s="74"/>
+      <c r="FO8" s="74"/>
+      <c r="FP8" s="74"/>
+      <c r="FQ8" s="74"/>
+      <c r="FR8" s="74"/>
+      <c r="FS8" s="74"/>
+      <c r="FT8" s="74"/>
+      <c r="FU8" s="74"/>
+      <c r="FV8" s="74"/>
+      <c r="FW8" s="74"/>
+      <c r="FX8" s="74"/>
+      <c r="FY8" s="74"/>
+      <c r="FZ8" s="74"/>
+      <c r="GA8" s="74"/>
+      <c r="GB8" s="74"/>
+      <c r="GC8" s="74"/>
+      <c r="GD8" s="74"/>
+      <c r="GE8" s="74"/>
+      <c r="GF8" s="74"/>
+      <c r="GG8" s="74"/>
+      <c r="GH8" s="74"/>
+      <c r="GI8" s="74"/>
+      <c r="GJ8" s="74"/>
+      <c r="GK8" s="74"/>
+      <c r="GL8" s="74"/>
+      <c r="GM8" s="74"/>
+      <c r="GN8" s="74"/>
+      <c r="GO8" s="74"/>
+      <c r="GP8" s="74"/>
+      <c r="GQ8" s="74"/>
+      <c r="GR8" s="74"/>
+      <c r="GS8" s="74"/>
+      <c r="GT8" s="74"/>
+      <c r="GU8" s="74"/>
+      <c r="GV8" s="74"/>
+      <c r="GW8" s="74"/>
+      <c r="GX8" s="74"/>
+      <c r="GY8" s="74"/>
+      <c r="GZ8" s="74"/>
+      <c r="HA8" s="74"/>
+      <c r="HB8" s="74"/>
+      <c r="HC8" s="74"/>
+      <c r="HD8" s="75"/>
+    </row>
+    <row r="9" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
@@ -2634,7 +3359,7 @@
       <c r="J9" s="46"/>
       <c r="K9" s="71"/>
     </row>
-    <row r="10" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
@@ -2646,7 +3371,7 @@
       <c r="J10" s="46"/>
       <c r="K10" s="71"/>
     </row>
-    <row r="11" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B11" s="32"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
@@ -2658,7 +3383,7 @@
       <c r="J11" s="46"/>
       <c r="K11" s="71"/>
     </row>
-    <row r="12" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B12" s="32"/>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
@@ -2670,7 +3395,7 @@
       <c r="J12" s="46"/>
       <c r="K12" s="71"/>
     </row>
-    <row r="13" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B13" s="32"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
@@ -2682,7 +3407,7 @@
       <c r="J13" s="46"/>
       <c r="K13" s="71"/>
     </row>
-    <row r="14" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
@@ -2694,7 +3419,7 @@
       <c r="J14" s="46"/>
       <c r="K14" s="71"/>
     </row>
-    <row r="15" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B15" s="32"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
@@ -2706,7 +3431,7 @@
       <c r="J15" s="46"/>
       <c r="K15" s="71"/>
     </row>
-    <row r="16" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B16" s="32"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
@@ -3210,7 +3935,7 @@
       <c r="J57" s="32"/>
       <c r="K57" s="71"/>
     </row>
-    <row r="1048575" spans="13:112" x14ac:dyDescent="0.25">
+    <row r="1048575" spans="13:212" x14ac:dyDescent="0.25">
       <c r="M1048575" s="48"/>
       <c r="N1048575" s="41"/>
       <c r="O1048575" s="41"/>
@@ -3310,15 +4035,115 @@
       <c r="DE1048575" s="41"/>
       <c r="DF1048575" s="41"/>
       <c r="DG1048575" s="41"/>
-      <c r="DH1048575" s="47"/>
+      <c r="DH1048575" s="41"/>
+      <c r="DI1048575" s="41"/>
+      <c r="DJ1048575" s="41"/>
+      <c r="DK1048575" s="41"/>
+      <c r="DL1048575" s="41"/>
+      <c r="DM1048575" s="41"/>
+      <c r="DN1048575" s="41"/>
+      <c r="DO1048575" s="41"/>
+      <c r="DP1048575" s="41"/>
+      <c r="DQ1048575" s="41"/>
+      <c r="DR1048575" s="41"/>
+      <c r="DS1048575" s="41"/>
+      <c r="DT1048575" s="41"/>
+      <c r="DU1048575" s="41"/>
+      <c r="DV1048575" s="41"/>
+      <c r="DW1048575" s="41"/>
+      <c r="DX1048575" s="41"/>
+      <c r="DY1048575" s="41"/>
+      <c r="DZ1048575" s="41"/>
+      <c r="EA1048575" s="41"/>
+      <c r="EB1048575" s="41"/>
+      <c r="EC1048575" s="41"/>
+      <c r="ED1048575" s="41"/>
+      <c r="EE1048575" s="41"/>
+      <c r="EF1048575" s="41"/>
+      <c r="EG1048575" s="41"/>
+      <c r="EH1048575" s="41"/>
+      <c r="EI1048575" s="41"/>
+      <c r="EJ1048575" s="41"/>
+      <c r="EK1048575" s="41"/>
+      <c r="EL1048575" s="41"/>
+      <c r="EM1048575" s="41"/>
+      <c r="EN1048575" s="41"/>
+      <c r="EO1048575" s="41"/>
+      <c r="EP1048575" s="41"/>
+      <c r="EQ1048575" s="41"/>
+      <c r="ER1048575" s="41"/>
+      <c r="ES1048575" s="41"/>
+      <c r="ET1048575" s="41"/>
+      <c r="EU1048575" s="41"/>
+      <c r="EV1048575" s="41"/>
+      <c r="EW1048575" s="41"/>
+      <c r="EX1048575" s="41"/>
+      <c r="EY1048575" s="41"/>
+      <c r="EZ1048575" s="41"/>
+      <c r="FA1048575" s="41"/>
+      <c r="FB1048575" s="41"/>
+      <c r="FC1048575" s="41"/>
+      <c r="FD1048575" s="41"/>
+      <c r="FE1048575" s="41"/>
+      <c r="FF1048575" s="41"/>
+      <c r="FG1048575" s="41"/>
+      <c r="FH1048575" s="41"/>
+      <c r="FI1048575" s="41"/>
+      <c r="FJ1048575" s="41"/>
+      <c r="FK1048575" s="41"/>
+      <c r="FL1048575" s="41"/>
+      <c r="FM1048575" s="41"/>
+      <c r="FN1048575" s="41"/>
+      <c r="FO1048575" s="41"/>
+      <c r="FP1048575" s="41"/>
+      <c r="FQ1048575" s="41"/>
+      <c r="FR1048575" s="41"/>
+      <c r="FS1048575" s="41"/>
+      <c r="FT1048575" s="41"/>
+      <c r="FU1048575" s="41"/>
+      <c r="FV1048575" s="41"/>
+      <c r="FW1048575" s="41"/>
+      <c r="FX1048575" s="41"/>
+      <c r="FY1048575" s="41"/>
+      <c r="FZ1048575" s="41"/>
+      <c r="GA1048575" s="41"/>
+      <c r="GB1048575" s="41"/>
+      <c r="GC1048575" s="41"/>
+      <c r="GD1048575" s="41"/>
+      <c r="GE1048575" s="41"/>
+      <c r="GF1048575" s="41"/>
+      <c r="GG1048575" s="41"/>
+      <c r="GH1048575" s="41"/>
+      <c r="GI1048575" s="41"/>
+      <c r="GJ1048575" s="41"/>
+      <c r="GK1048575" s="41"/>
+      <c r="GL1048575" s="41"/>
+      <c r="GM1048575" s="41"/>
+      <c r="GN1048575" s="41"/>
+      <c r="GO1048575" s="41"/>
+      <c r="GP1048575" s="41"/>
+      <c r="GQ1048575" s="41"/>
+      <c r="GR1048575" s="41"/>
+      <c r="GS1048575" s="41"/>
+      <c r="GT1048575" s="41"/>
+      <c r="GU1048575" s="41"/>
+      <c r="GV1048575" s="41"/>
+      <c r="GW1048575" s="41"/>
+      <c r="GX1048575" s="41"/>
+      <c r="GY1048575" s="41"/>
+      <c r="GZ1048575" s="41"/>
+      <c r="HA1048575" s="41"/>
+      <c r="HB1048575" s="41"/>
+      <c r="HC1048575" s="41"/>
+      <c r="HD1048575" s="47"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="j0NcjX851y4PtVYbj98JVHZcIL0PetLE4dhGwBaUCSDiCl+UeH0eLW/8sJLso5EcCoerD4+55D7C3sHDpH2Tog==" saltValue="fbiOfWctC0fVsFWxS5e+Sw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vDsptiMRF8QIMLQpO3bZ1sESTVpUW1Hqfu69+NtC+0Eyc+2i6AnjikbLjmv8FUjGldUyruu0Rz2IoXDrFMQOYw==" saltValue="zXAfBtdGoej2q4pHRntN/Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="B4:F6"/>
     <mergeCell ref="G4:I6"/>
     <mergeCell ref="J4:K6"/>
-    <mergeCell ref="M3:DH3"/>
+    <mergeCell ref="M3:HD3"/>
     <mergeCell ref="B2:K3"/>
     <mergeCell ref="L2:L3"/>
   </mergeCells>
@@ -3327,7 +4152,7 @@
       <formula>B8=""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8:DH1048576">
+  <conditionalFormatting sqref="M8:HD1048576">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>M8=""</formula>
     </cfRule>

</xml_diff>

<commit_message>
Showing rows / columns on Data worksheet
</commit_message>
<xml_diff>
--- a/forms/Form-1DI.xlsx
+++ b/forms/Form-1DI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C52E6CE-4789-463C-8AB3-F372674CFA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A65E2AB-A8EE-4794-B77E-064EE801ABA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -1788,7 +1788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:HD1048575"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="12" ySplit="7" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>

</xml_diff>

<commit_message>
Fixing link to condition at release
</commit_message>
<xml_diff>
--- a/forms/Form-1DI.xlsx
+++ b/forms/Form-1DI.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A65E2AB-A8EE-4794-B77E-064EE801ABA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1FB030-0581-4D2D-90F2-C8C9F03955A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -795,7 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -977,10 +977,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1496,24 +1492,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="87"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="90"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="89"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -1563,15 +1559,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="84"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="84" t="s">
+      <c r="F8" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="84"/>
+      <c r="G8" s="83"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1742,11 +1738,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="83"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1798,19 +1794,19 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="66" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" style="67" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="67" customWidth="1"/>
-    <col min="6" max="6" width="14" style="68" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="66" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="67" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="69" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="66" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="72" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="76"/>
-    <col min="14" max="211" width="9.140625" style="77"/>
-    <col min="212" max="212" width="9.140625" style="78"/>
+    <col min="2" max="2" width="11.42578125" style="65" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" style="66" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="66" customWidth="1"/>
+    <col min="6" max="6" width="14" style="67" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="65" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="66" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="68" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="65" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="71" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="79" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="75"/>
+    <col min="14" max="211" width="9.140625" style="76"/>
+    <col min="212" max="212" width="9.140625" style="77"/>
     <col min="213" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
@@ -1818,19 +1814,19 @@
       <c r="K1" s="38"/>
     </row>
     <row r="2" spans="1:212" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="112"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="111"/>
       <c r="M2" s="35"/>
       <c r="N2" s="35"/>
       <c r="O2" s="35"/>
@@ -2034,237 +2030,237 @@
     </row>
     <row r="3" spans="1:212" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="113"/>
-      <c r="M3" s="109" t="s">
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="108" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="110"/>
-      <c r="O3" s="110"/>
-      <c r="P3" s="110"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="110"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="110"/>
-      <c r="U3" s="110"/>
-      <c r="V3" s="110"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="110"/>
-      <c r="Y3" s="110"/>
-      <c r="Z3" s="110"/>
-      <c r="AA3" s="110"/>
-      <c r="AB3" s="110"/>
-      <c r="AC3" s="110"/>
-      <c r="AD3" s="110"/>
-      <c r="AE3" s="110"/>
-      <c r="AF3" s="110"/>
-      <c r="AG3" s="110"/>
-      <c r="AH3" s="110"/>
-      <c r="AI3" s="110"/>
-      <c r="AJ3" s="110"/>
-      <c r="AK3" s="110"/>
-      <c r="AL3" s="110"/>
-      <c r="AM3" s="110"/>
-      <c r="AN3" s="110"/>
-      <c r="AO3" s="110"/>
-      <c r="AP3" s="110"/>
-      <c r="AQ3" s="110"/>
-      <c r="AR3" s="110"/>
-      <c r="AS3" s="110"/>
-      <c r="AT3" s="110"/>
-      <c r="AU3" s="110"/>
-      <c r="AV3" s="110"/>
-      <c r="AW3" s="110"/>
-      <c r="AX3" s="110"/>
-      <c r="AY3" s="110"/>
-      <c r="AZ3" s="110"/>
-      <c r="BA3" s="110"/>
-      <c r="BB3" s="110"/>
-      <c r="BC3" s="110"/>
-      <c r="BD3" s="110"/>
-      <c r="BE3" s="110"/>
-      <c r="BF3" s="110"/>
-      <c r="BG3" s="110"/>
-      <c r="BH3" s="110"/>
-      <c r="BI3" s="110"/>
-      <c r="BJ3" s="110"/>
-      <c r="BK3" s="110"/>
-      <c r="BL3" s="110"/>
-      <c r="BM3" s="110"/>
-      <c r="BN3" s="110"/>
-      <c r="BO3" s="110"/>
-      <c r="BP3" s="110"/>
-      <c r="BQ3" s="110"/>
-      <c r="BR3" s="110"/>
-      <c r="BS3" s="110"/>
-      <c r="BT3" s="110"/>
-      <c r="BU3" s="110"/>
-      <c r="BV3" s="110"/>
-      <c r="BW3" s="110"/>
-      <c r="BX3" s="110"/>
-      <c r="BY3" s="110"/>
-      <c r="BZ3" s="110"/>
-      <c r="CA3" s="110"/>
-      <c r="CB3" s="110"/>
-      <c r="CC3" s="110"/>
-      <c r="CD3" s="110"/>
-      <c r="CE3" s="110"/>
-      <c r="CF3" s="110"/>
-      <c r="CG3" s="110"/>
-      <c r="CH3" s="110"/>
-      <c r="CI3" s="110"/>
-      <c r="CJ3" s="110"/>
-      <c r="CK3" s="110"/>
-      <c r="CL3" s="110"/>
-      <c r="CM3" s="110"/>
-      <c r="CN3" s="110"/>
-      <c r="CO3" s="110"/>
-      <c r="CP3" s="110"/>
-      <c r="CQ3" s="110"/>
-      <c r="CR3" s="110"/>
-      <c r="CS3" s="110"/>
-      <c r="CT3" s="110"/>
-      <c r="CU3" s="110"/>
-      <c r="CV3" s="110"/>
-      <c r="CW3" s="110"/>
-      <c r="CX3" s="110"/>
-      <c r="CY3" s="110"/>
-      <c r="CZ3" s="110"/>
-      <c r="DA3" s="110"/>
-      <c r="DB3" s="110"/>
-      <c r="DC3" s="110"/>
-      <c r="DD3" s="110"/>
-      <c r="DE3" s="110"/>
-      <c r="DF3" s="110"/>
-      <c r="DG3" s="110"/>
-      <c r="DH3" s="110"/>
-      <c r="DI3" s="110"/>
-      <c r="DJ3" s="110"/>
-      <c r="DK3" s="110"/>
-      <c r="DL3" s="110"/>
-      <c r="DM3" s="110"/>
-      <c r="DN3" s="110"/>
-      <c r="DO3" s="110"/>
-      <c r="DP3" s="110"/>
-      <c r="DQ3" s="110"/>
-      <c r="DR3" s="110"/>
-      <c r="DS3" s="110"/>
-      <c r="DT3" s="110"/>
-      <c r="DU3" s="110"/>
-      <c r="DV3" s="110"/>
-      <c r="DW3" s="110"/>
-      <c r="DX3" s="110"/>
-      <c r="DY3" s="110"/>
-      <c r="DZ3" s="110"/>
-      <c r="EA3" s="110"/>
-      <c r="EB3" s="110"/>
-      <c r="EC3" s="110"/>
-      <c r="ED3" s="110"/>
-      <c r="EE3" s="110"/>
-      <c r="EF3" s="110"/>
-      <c r="EG3" s="110"/>
-      <c r="EH3" s="110"/>
-      <c r="EI3" s="110"/>
-      <c r="EJ3" s="110"/>
-      <c r="EK3" s="110"/>
-      <c r="EL3" s="110"/>
-      <c r="EM3" s="110"/>
-      <c r="EN3" s="110"/>
-      <c r="EO3" s="110"/>
-      <c r="EP3" s="110"/>
-      <c r="EQ3" s="110"/>
-      <c r="ER3" s="110"/>
-      <c r="ES3" s="110"/>
-      <c r="ET3" s="110"/>
-      <c r="EU3" s="110"/>
-      <c r="EV3" s="110"/>
-      <c r="EW3" s="110"/>
-      <c r="EX3" s="110"/>
-      <c r="EY3" s="110"/>
-      <c r="EZ3" s="110"/>
-      <c r="FA3" s="110"/>
-      <c r="FB3" s="110"/>
-      <c r="FC3" s="110"/>
-      <c r="FD3" s="110"/>
-      <c r="FE3" s="110"/>
-      <c r="FF3" s="110"/>
-      <c r="FG3" s="110"/>
-      <c r="FH3" s="110"/>
-      <c r="FI3" s="110"/>
-      <c r="FJ3" s="110"/>
-      <c r="FK3" s="110"/>
-      <c r="FL3" s="110"/>
-      <c r="FM3" s="110"/>
-      <c r="FN3" s="110"/>
-      <c r="FO3" s="110"/>
-      <c r="FP3" s="110"/>
-      <c r="FQ3" s="110"/>
-      <c r="FR3" s="110"/>
-      <c r="FS3" s="110"/>
-      <c r="FT3" s="110"/>
-      <c r="FU3" s="110"/>
-      <c r="FV3" s="110"/>
-      <c r="FW3" s="110"/>
-      <c r="FX3" s="110"/>
-      <c r="FY3" s="110"/>
-      <c r="FZ3" s="110"/>
-      <c r="GA3" s="110"/>
-      <c r="GB3" s="110"/>
-      <c r="GC3" s="110"/>
-      <c r="GD3" s="110"/>
-      <c r="GE3" s="110"/>
-      <c r="GF3" s="110"/>
-      <c r="GG3" s="110"/>
-      <c r="GH3" s="110"/>
-      <c r="GI3" s="110"/>
-      <c r="GJ3" s="110"/>
-      <c r="GK3" s="110"/>
-      <c r="GL3" s="110"/>
-      <c r="GM3" s="110"/>
-      <c r="GN3" s="110"/>
-      <c r="GO3" s="110"/>
-      <c r="GP3" s="110"/>
-      <c r="GQ3" s="110"/>
-      <c r="GR3" s="110"/>
-      <c r="GS3" s="110"/>
-      <c r="GT3" s="110"/>
-      <c r="GU3" s="110"/>
-      <c r="GV3" s="110"/>
-      <c r="GW3" s="110"/>
-      <c r="GX3" s="110"/>
-      <c r="GY3" s="110"/>
-      <c r="GZ3" s="110"/>
-      <c r="HA3" s="110"/>
-      <c r="HB3" s="110"/>
-      <c r="HC3" s="110"/>
-      <c r="HD3" s="111"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
+      <c r="AB3" s="109"/>
+      <c r="AC3" s="109"/>
+      <c r="AD3" s="109"/>
+      <c r="AE3" s="109"/>
+      <c r="AF3" s="109"/>
+      <c r="AG3" s="109"/>
+      <c r="AH3" s="109"/>
+      <c r="AI3" s="109"/>
+      <c r="AJ3" s="109"/>
+      <c r="AK3" s="109"/>
+      <c r="AL3" s="109"/>
+      <c r="AM3" s="109"/>
+      <c r="AN3" s="109"/>
+      <c r="AO3" s="109"/>
+      <c r="AP3" s="109"/>
+      <c r="AQ3" s="109"/>
+      <c r="AR3" s="109"/>
+      <c r="AS3" s="109"/>
+      <c r="AT3" s="109"/>
+      <c r="AU3" s="109"/>
+      <c r="AV3" s="109"/>
+      <c r="AW3" s="109"/>
+      <c r="AX3" s="109"/>
+      <c r="AY3" s="109"/>
+      <c r="AZ3" s="109"/>
+      <c r="BA3" s="109"/>
+      <c r="BB3" s="109"/>
+      <c r="BC3" s="109"/>
+      <c r="BD3" s="109"/>
+      <c r="BE3" s="109"/>
+      <c r="BF3" s="109"/>
+      <c r="BG3" s="109"/>
+      <c r="BH3" s="109"/>
+      <c r="BI3" s="109"/>
+      <c r="BJ3" s="109"/>
+      <c r="BK3" s="109"/>
+      <c r="BL3" s="109"/>
+      <c r="BM3" s="109"/>
+      <c r="BN3" s="109"/>
+      <c r="BO3" s="109"/>
+      <c r="BP3" s="109"/>
+      <c r="BQ3" s="109"/>
+      <c r="BR3" s="109"/>
+      <c r="BS3" s="109"/>
+      <c r="BT3" s="109"/>
+      <c r="BU3" s="109"/>
+      <c r="BV3" s="109"/>
+      <c r="BW3" s="109"/>
+      <c r="BX3" s="109"/>
+      <c r="BY3" s="109"/>
+      <c r="BZ3" s="109"/>
+      <c r="CA3" s="109"/>
+      <c r="CB3" s="109"/>
+      <c r="CC3" s="109"/>
+      <c r="CD3" s="109"/>
+      <c r="CE3" s="109"/>
+      <c r="CF3" s="109"/>
+      <c r="CG3" s="109"/>
+      <c r="CH3" s="109"/>
+      <c r="CI3" s="109"/>
+      <c r="CJ3" s="109"/>
+      <c r="CK3" s="109"/>
+      <c r="CL3" s="109"/>
+      <c r="CM3" s="109"/>
+      <c r="CN3" s="109"/>
+      <c r="CO3" s="109"/>
+      <c r="CP3" s="109"/>
+      <c r="CQ3" s="109"/>
+      <c r="CR3" s="109"/>
+      <c r="CS3" s="109"/>
+      <c r="CT3" s="109"/>
+      <c r="CU3" s="109"/>
+      <c r="CV3" s="109"/>
+      <c r="CW3" s="109"/>
+      <c r="CX3" s="109"/>
+      <c r="CY3" s="109"/>
+      <c r="CZ3" s="109"/>
+      <c r="DA3" s="109"/>
+      <c r="DB3" s="109"/>
+      <c r="DC3" s="109"/>
+      <c r="DD3" s="109"/>
+      <c r="DE3" s="109"/>
+      <c r="DF3" s="109"/>
+      <c r="DG3" s="109"/>
+      <c r="DH3" s="109"/>
+      <c r="DI3" s="109"/>
+      <c r="DJ3" s="109"/>
+      <c r="DK3" s="109"/>
+      <c r="DL3" s="109"/>
+      <c r="DM3" s="109"/>
+      <c r="DN3" s="109"/>
+      <c r="DO3" s="109"/>
+      <c r="DP3" s="109"/>
+      <c r="DQ3" s="109"/>
+      <c r="DR3" s="109"/>
+      <c r="DS3" s="109"/>
+      <c r="DT3" s="109"/>
+      <c r="DU3" s="109"/>
+      <c r="DV3" s="109"/>
+      <c r="DW3" s="109"/>
+      <c r="DX3" s="109"/>
+      <c r="DY3" s="109"/>
+      <c r="DZ3" s="109"/>
+      <c r="EA3" s="109"/>
+      <c r="EB3" s="109"/>
+      <c r="EC3" s="109"/>
+      <c r="ED3" s="109"/>
+      <c r="EE3" s="109"/>
+      <c r="EF3" s="109"/>
+      <c r="EG3" s="109"/>
+      <c r="EH3" s="109"/>
+      <c r="EI3" s="109"/>
+      <c r="EJ3" s="109"/>
+      <c r="EK3" s="109"/>
+      <c r="EL3" s="109"/>
+      <c r="EM3" s="109"/>
+      <c r="EN3" s="109"/>
+      <c r="EO3" s="109"/>
+      <c r="EP3" s="109"/>
+      <c r="EQ3" s="109"/>
+      <c r="ER3" s="109"/>
+      <c r="ES3" s="109"/>
+      <c r="ET3" s="109"/>
+      <c r="EU3" s="109"/>
+      <c r="EV3" s="109"/>
+      <c r="EW3" s="109"/>
+      <c r="EX3" s="109"/>
+      <c r="EY3" s="109"/>
+      <c r="EZ3" s="109"/>
+      <c r="FA3" s="109"/>
+      <c r="FB3" s="109"/>
+      <c r="FC3" s="109"/>
+      <c r="FD3" s="109"/>
+      <c r="FE3" s="109"/>
+      <c r="FF3" s="109"/>
+      <c r="FG3" s="109"/>
+      <c r="FH3" s="109"/>
+      <c r="FI3" s="109"/>
+      <c r="FJ3" s="109"/>
+      <c r="FK3" s="109"/>
+      <c r="FL3" s="109"/>
+      <c r="FM3" s="109"/>
+      <c r="FN3" s="109"/>
+      <c r="FO3" s="109"/>
+      <c r="FP3" s="109"/>
+      <c r="FQ3" s="109"/>
+      <c r="FR3" s="109"/>
+      <c r="FS3" s="109"/>
+      <c r="FT3" s="109"/>
+      <c r="FU3" s="109"/>
+      <c r="FV3" s="109"/>
+      <c r="FW3" s="109"/>
+      <c r="FX3" s="109"/>
+      <c r="FY3" s="109"/>
+      <c r="FZ3" s="109"/>
+      <c r="GA3" s="109"/>
+      <c r="GB3" s="109"/>
+      <c r="GC3" s="109"/>
+      <c r="GD3" s="109"/>
+      <c r="GE3" s="109"/>
+      <c r="GF3" s="109"/>
+      <c r="GG3" s="109"/>
+      <c r="GH3" s="109"/>
+      <c r="GI3" s="109"/>
+      <c r="GJ3" s="109"/>
+      <c r="GK3" s="109"/>
+      <c r="GL3" s="109"/>
+      <c r="GM3" s="109"/>
+      <c r="GN3" s="109"/>
+      <c r="GO3" s="109"/>
+      <c r="GP3" s="109"/>
+      <c r="GQ3" s="109"/>
+      <c r="GR3" s="109"/>
+      <c r="GS3" s="109"/>
+      <c r="GT3" s="109"/>
+      <c r="GU3" s="109"/>
+      <c r="GV3" s="109"/>
+      <c r="GW3" s="109"/>
+      <c r="GX3" s="109"/>
+      <c r="GY3" s="109"/>
+      <c r="GZ3" s="109"/>
+      <c r="HA3" s="109"/>
+      <c r="HB3" s="109"/>
+      <c r="HC3" s="109"/>
+      <c r="HD3" s="110"/>
     </row>
     <row r="4" spans="1:212" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="100" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="101"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="100" t="s">
+      <c r="H4" s="100"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="102"/>
+      <c r="K4" s="101"/>
       <c r="L4" s="63" t="s">
         <v>16</v>
       </c>
@@ -2470,17 +2466,17 @@
       <c r="HD4" s="28"/>
     </row>
     <row r="5" spans="1:212" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="94"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="103"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="64" t="s">
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="102"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="51" t="s">
         <v>15</v>
       </c>
       <c r="M5" s="26"/>
@@ -2685,16 +2681,16 @@
       <c r="HD5" s="28"/>
     </row>
     <row r="6" spans="1:212" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="97"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="108"/>
-      <c r="J6" s="106"/>
-      <c r="K6" s="108"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="107"/>
       <c r="L6" s="51" t="s">
         <v>26</v>
       </c>
@@ -2930,7 +2926,7 @@
       <c r="K7" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="65" t="s">
+      <c r="L7" s="64" t="s">
         <v>32</v>
       </c>
       <c r="M7" s="29"/>
@@ -3144,208 +3140,208 @@
       <c r="H8" s="43"/>
       <c r="I8" s="44"/>
       <c r="J8" s="45"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-      <c r="S8" s="74"/>
-      <c r="T8" s="74"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="74"/>
-      <c r="W8" s="74"/>
-      <c r="X8" s="74"/>
-      <c r="Y8" s="74"/>
-      <c r="Z8" s="74"/>
-      <c r="AA8" s="74"/>
-      <c r="AB8" s="74"/>
-      <c r="AC8" s="74"/>
-      <c r="AD8" s="74"/>
-      <c r="AE8" s="74"/>
-      <c r="AF8" s="74"/>
-      <c r="AG8" s="74"/>
-      <c r="AH8" s="74"/>
-      <c r="AI8" s="74"/>
-      <c r="AJ8" s="74"/>
-      <c r="AK8" s="74"/>
-      <c r="AL8" s="74"/>
-      <c r="AM8" s="74"/>
-      <c r="AN8" s="74"/>
-      <c r="AO8" s="74"/>
-      <c r="AP8" s="74"/>
-      <c r="AQ8" s="74"/>
-      <c r="AR8" s="74"/>
-      <c r="AS8" s="74"/>
-      <c r="AT8" s="74"/>
-      <c r="AU8" s="74"/>
-      <c r="AV8" s="74"/>
-      <c r="AW8" s="74"/>
-      <c r="AX8" s="74"/>
-      <c r="AY8" s="74"/>
-      <c r="AZ8" s="74"/>
-      <c r="BA8" s="74"/>
-      <c r="BB8" s="74"/>
-      <c r="BC8" s="74"/>
-      <c r="BD8" s="74"/>
-      <c r="BE8" s="74"/>
-      <c r="BF8" s="74"/>
-      <c r="BG8" s="74"/>
-      <c r="BH8" s="74"/>
-      <c r="BI8" s="74"/>
-      <c r="BJ8" s="74"/>
-      <c r="BK8" s="74"/>
-      <c r="BL8" s="74"/>
-      <c r="BM8" s="74"/>
-      <c r="BN8" s="74"/>
-      <c r="BO8" s="74"/>
-      <c r="BP8" s="74"/>
-      <c r="BQ8" s="74"/>
-      <c r="BR8" s="74"/>
-      <c r="BS8" s="74"/>
-      <c r="BT8" s="74"/>
-      <c r="BU8" s="74"/>
-      <c r="BV8" s="74"/>
-      <c r="BW8" s="74"/>
-      <c r="BX8" s="74"/>
-      <c r="BY8" s="74"/>
-      <c r="BZ8" s="74"/>
-      <c r="CA8" s="74"/>
-      <c r="CB8" s="74"/>
-      <c r="CC8" s="74"/>
-      <c r="CD8" s="74"/>
-      <c r="CE8" s="74"/>
-      <c r="CF8" s="74"/>
-      <c r="CG8" s="74"/>
-      <c r="CH8" s="74"/>
-      <c r="CI8" s="74"/>
-      <c r="CJ8" s="74"/>
-      <c r="CK8" s="74"/>
-      <c r="CL8" s="74"/>
-      <c r="CM8" s="74"/>
-      <c r="CN8" s="74"/>
-      <c r="CO8" s="74"/>
-      <c r="CP8" s="74"/>
-      <c r="CQ8" s="74"/>
-      <c r="CR8" s="74"/>
-      <c r="CS8" s="74"/>
-      <c r="CT8" s="74"/>
-      <c r="CU8" s="74"/>
-      <c r="CV8" s="74"/>
-      <c r="CW8" s="74"/>
-      <c r="CX8" s="74"/>
-      <c r="CY8" s="74"/>
-      <c r="CZ8" s="74"/>
-      <c r="DA8" s="74"/>
-      <c r="DB8" s="74"/>
-      <c r="DC8" s="74"/>
-      <c r="DD8" s="74"/>
-      <c r="DE8" s="74"/>
-      <c r="DF8" s="74"/>
-      <c r="DG8" s="74"/>
-      <c r="DH8" s="74"/>
-      <c r="DI8" s="74"/>
-      <c r="DJ8" s="74"/>
-      <c r="DK8" s="74"/>
-      <c r="DL8" s="74"/>
-      <c r="DM8" s="74"/>
-      <c r="DN8" s="74"/>
-      <c r="DO8" s="74"/>
-      <c r="DP8" s="74"/>
-      <c r="DQ8" s="74"/>
-      <c r="DR8" s="74"/>
-      <c r="DS8" s="74"/>
-      <c r="DT8" s="74"/>
-      <c r="DU8" s="74"/>
-      <c r="DV8" s="74"/>
-      <c r="DW8" s="74"/>
-      <c r="DX8" s="74"/>
-      <c r="DY8" s="74"/>
-      <c r="DZ8" s="74"/>
-      <c r="EA8" s="74"/>
-      <c r="EB8" s="74"/>
-      <c r="EC8" s="74"/>
-      <c r="ED8" s="74"/>
-      <c r="EE8" s="74"/>
-      <c r="EF8" s="74"/>
-      <c r="EG8" s="74"/>
-      <c r="EH8" s="74"/>
-      <c r="EI8" s="74"/>
-      <c r="EJ8" s="74"/>
-      <c r="EK8" s="74"/>
-      <c r="EL8" s="74"/>
-      <c r="EM8" s="74"/>
-      <c r="EN8" s="74"/>
-      <c r="EO8" s="74"/>
-      <c r="EP8" s="74"/>
-      <c r="EQ8" s="74"/>
-      <c r="ER8" s="74"/>
-      <c r="ES8" s="74"/>
-      <c r="ET8" s="74"/>
-      <c r="EU8" s="74"/>
-      <c r="EV8" s="74"/>
-      <c r="EW8" s="74"/>
-      <c r="EX8" s="74"/>
-      <c r="EY8" s="74"/>
-      <c r="EZ8" s="74"/>
-      <c r="FA8" s="74"/>
-      <c r="FB8" s="74"/>
-      <c r="FC8" s="74"/>
-      <c r="FD8" s="74"/>
-      <c r="FE8" s="74"/>
-      <c r="FF8" s="74"/>
-      <c r="FG8" s="74"/>
-      <c r="FH8" s="74"/>
-      <c r="FI8" s="74"/>
-      <c r="FJ8" s="74"/>
-      <c r="FK8" s="74"/>
-      <c r="FL8" s="74"/>
-      <c r="FM8" s="74"/>
-      <c r="FN8" s="74"/>
-      <c r="FO8" s="74"/>
-      <c r="FP8" s="74"/>
-      <c r="FQ8" s="74"/>
-      <c r="FR8" s="74"/>
-      <c r="FS8" s="74"/>
-      <c r="FT8" s="74"/>
-      <c r="FU8" s="74"/>
-      <c r="FV8" s="74"/>
-      <c r="FW8" s="74"/>
-      <c r="FX8" s="74"/>
-      <c r="FY8" s="74"/>
-      <c r="FZ8" s="74"/>
-      <c r="GA8" s="74"/>
-      <c r="GB8" s="74"/>
-      <c r="GC8" s="74"/>
-      <c r="GD8" s="74"/>
-      <c r="GE8" s="74"/>
-      <c r="GF8" s="74"/>
-      <c r="GG8" s="74"/>
-      <c r="GH8" s="74"/>
-      <c r="GI8" s="74"/>
-      <c r="GJ8" s="74"/>
-      <c r="GK8" s="74"/>
-      <c r="GL8" s="74"/>
-      <c r="GM8" s="74"/>
-      <c r="GN8" s="74"/>
-      <c r="GO8" s="74"/>
-      <c r="GP8" s="74"/>
-      <c r="GQ8" s="74"/>
-      <c r="GR8" s="74"/>
-      <c r="GS8" s="74"/>
-      <c r="GT8" s="74"/>
-      <c r="GU8" s="74"/>
-      <c r="GV8" s="74"/>
-      <c r="GW8" s="74"/>
-      <c r="GX8" s="74"/>
-      <c r="GY8" s="74"/>
-      <c r="GZ8" s="74"/>
-      <c r="HA8" s="74"/>
-      <c r="HB8" s="74"/>
-      <c r="HC8" s="74"/>
-      <c r="HD8" s="75"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="73"/>
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="73"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="73"/>
+      <c r="V8" s="73"/>
+      <c r="W8" s="73"/>
+      <c r="X8" s="73"/>
+      <c r="Y8" s="73"/>
+      <c r="Z8" s="73"/>
+      <c r="AA8" s="73"/>
+      <c r="AB8" s="73"/>
+      <c r="AC8" s="73"/>
+      <c r="AD8" s="73"/>
+      <c r="AE8" s="73"/>
+      <c r="AF8" s="73"/>
+      <c r="AG8" s="73"/>
+      <c r="AH8" s="73"/>
+      <c r="AI8" s="73"/>
+      <c r="AJ8" s="73"/>
+      <c r="AK8" s="73"/>
+      <c r="AL8" s="73"/>
+      <c r="AM8" s="73"/>
+      <c r="AN8" s="73"/>
+      <c r="AO8" s="73"/>
+      <c r="AP8" s="73"/>
+      <c r="AQ8" s="73"/>
+      <c r="AR8" s="73"/>
+      <c r="AS8" s="73"/>
+      <c r="AT8" s="73"/>
+      <c r="AU8" s="73"/>
+      <c r="AV8" s="73"/>
+      <c r="AW8" s="73"/>
+      <c r="AX8" s="73"/>
+      <c r="AY8" s="73"/>
+      <c r="AZ8" s="73"/>
+      <c r="BA8" s="73"/>
+      <c r="BB8" s="73"/>
+      <c r="BC8" s="73"/>
+      <c r="BD8" s="73"/>
+      <c r="BE8" s="73"/>
+      <c r="BF8" s="73"/>
+      <c r="BG8" s="73"/>
+      <c r="BH8" s="73"/>
+      <c r="BI8" s="73"/>
+      <c r="BJ8" s="73"/>
+      <c r="BK8" s="73"/>
+      <c r="BL8" s="73"/>
+      <c r="BM8" s="73"/>
+      <c r="BN8" s="73"/>
+      <c r="BO8" s="73"/>
+      <c r="BP8" s="73"/>
+      <c r="BQ8" s="73"/>
+      <c r="BR8" s="73"/>
+      <c r="BS8" s="73"/>
+      <c r="BT8" s="73"/>
+      <c r="BU8" s="73"/>
+      <c r="BV8" s="73"/>
+      <c r="BW8" s="73"/>
+      <c r="BX8" s="73"/>
+      <c r="BY8" s="73"/>
+      <c r="BZ8" s="73"/>
+      <c r="CA8" s="73"/>
+      <c r="CB8" s="73"/>
+      <c r="CC8" s="73"/>
+      <c r="CD8" s="73"/>
+      <c r="CE8" s="73"/>
+      <c r="CF8" s="73"/>
+      <c r="CG8" s="73"/>
+      <c r="CH8" s="73"/>
+      <c r="CI8" s="73"/>
+      <c r="CJ8" s="73"/>
+      <c r="CK8" s="73"/>
+      <c r="CL8" s="73"/>
+      <c r="CM8" s="73"/>
+      <c r="CN8" s="73"/>
+      <c r="CO8" s="73"/>
+      <c r="CP8" s="73"/>
+      <c r="CQ8" s="73"/>
+      <c r="CR8" s="73"/>
+      <c r="CS8" s="73"/>
+      <c r="CT8" s="73"/>
+      <c r="CU8" s="73"/>
+      <c r="CV8" s="73"/>
+      <c r="CW8" s="73"/>
+      <c r="CX8" s="73"/>
+      <c r="CY8" s="73"/>
+      <c r="CZ8" s="73"/>
+      <c r="DA8" s="73"/>
+      <c r="DB8" s="73"/>
+      <c r="DC8" s="73"/>
+      <c r="DD8" s="73"/>
+      <c r="DE8" s="73"/>
+      <c r="DF8" s="73"/>
+      <c r="DG8" s="73"/>
+      <c r="DH8" s="73"/>
+      <c r="DI8" s="73"/>
+      <c r="DJ8" s="73"/>
+      <c r="DK8" s="73"/>
+      <c r="DL8" s="73"/>
+      <c r="DM8" s="73"/>
+      <c r="DN8" s="73"/>
+      <c r="DO8" s="73"/>
+      <c r="DP8" s="73"/>
+      <c r="DQ8" s="73"/>
+      <c r="DR8" s="73"/>
+      <c r="DS8" s="73"/>
+      <c r="DT8" s="73"/>
+      <c r="DU8" s="73"/>
+      <c r="DV8" s="73"/>
+      <c r="DW8" s="73"/>
+      <c r="DX8" s="73"/>
+      <c r="DY8" s="73"/>
+      <c r="DZ8" s="73"/>
+      <c r="EA8" s="73"/>
+      <c r="EB8" s="73"/>
+      <c r="EC8" s="73"/>
+      <c r="ED8" s="73"/>
+      <c r="EE8" s="73"/>
+      <c r="EF8" s="73"/>
+      <c r="EG8" s="73"/>
+      <c r="EH8" s="73"/>
+      <c r="EI8" s="73"/>
+      <c r="EJ8" s="73"/>
+      <c r="EK8" s="73"/>
+      <c r="EL8" s="73"/>
+      <c r="EM8" s="73"/>
+      <c r="EN8" s="73"/>
+      <c r="EO8" s="73"/>
+      <c r="EP8" s="73"/>
+      <c r="EQ8" s="73"/>
+      <c r="ER8" s="73"/>
+      <c r="ES8" s="73"/>
+      <c r="ET8" s="73"/>
+      <c r="EU8" s="73"/>
+      <c r="EV8" s="73"/>
+      <c r="EW8" s="73"/>
+      <c r="EX8" s="73"/>
+      <c r="EY8" s="73"/>
+      <c r="EZ8" s="73"/>
+      <c r="FA8" s="73"/>
+      <c r="FB8" s="73"/>
+      <c r="FC8" s="73"/>
+      <c r="FD8" s="73"/>
+      <c r="FE8" s="73"/>
+      <c r="FF8" s="73"/>
+      <c r="FG8" s="73"/>
+      <c r="FH8" s="73"/>
+      <c r="FI8" s="73"/>
+      <c r="FJ8" s="73"/>
+      <c r="FK8" s="73"/>
+      <c r="FL8" s="73"/>
+      <c r="FM8" s="73"/>
+      <c r="FN8" s="73"/>
+      <c r="FO8" s="73"/>
+      <c r="FP8" s="73"/>
+      <c r="FQ8" s="73"/>
+      <c r="FR8" s="73"/>
+      <c r="FS8" s="73"/>
+      <c r="FT8" s="73"/>
+      <c r="FU8" s="73"/>
+      <c r="FV8" s="73"/>
+      <c r="FW8" s="73"/>
+      <c r="FX8" s="73"/>
+      <c r="FY8" s="73"/>
+      <c r="FZ8" s="73"/>
+      <c r="GA8" s="73"/>
+      <c r="GB8" s="73"/>
+      <c r="GC8" s="73"/>
+      <c r="GD8" s="73"/>
+      <c r="GE8" s="73"/>
+      <c r="GF8" s="73"/>
+      <c r="GG8" s="73"/>
+      <c r="GH8" s="73"/>
+      <c r="GI8" s="73"/>
+      <c r="GJ8" s="73"/>
+      <c r="GK8" s="73"/>
+      <c r="GL8" s="73"/>
+      <c r="GM8" s="73"/>
+      <c r="GN8" s="73"/>
+      <c r="GO8" s="73"/>
+      <c r="GP8" s="73"/>
+      <c r="GQ8" s="73"/>
+      <c r="GR8" s="73"/>
+      <c r="GS8" s="73"/>
+      <c r="GT8" s="73"/>
+      <c r="GU8" s="73"/>
+      <c r="GV8" s="73"/>
+      <c r="GW8" s="73"/>
+      <c r="GX8" s="73"/>
+      <c r="GY8" s="73"/>
+      <c r="GZ8" s="73"/>
+      <c r="HA8" s="73"/>
+      <c r="HB8" s="73"/>
+      <c r="HC8" s="73"/>
+      <c r="HD8" s="74"/>
     </row>
     <row r="9" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
@@ -3357,7 +3353,7 @@
       <c r="H9" s="33"/>
       <c r="I9" s="34"/>
       <c r="J9" s="46"/>
-      <c r="K9" s="71"/>
+      <c r="K9" s="70"/>
     </row>
     <row r="10" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
@@ -3369,7 +3365,7 @@
       <c r="H10" s="33"/>
       <c r="I10" s="34"/>
       <c r="J10" s="46"/>
-      <c r="K10" s="71"/>
+      <c r="K10" s="70"/>
     </row>
     <row r="11" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B11" s="32"/>
@@ -3381,7 +3377,7 @@
       <c r="H11" s="33"/>
       <c r="I11" s="34"/>
       <c r="J11" s="46"/>
-      <c r="K11" s="71"/>
+      <c r="K11" s="70"/>
     </row>
     <row r="12" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B12" s="32"/>
@@ -3393,7 +3389,7 @@
       <c r="H12" s="33"/>
       <c r="I12" s="34"/>
       <c r="J12" s="46"/>
-      <c r="K12" s="71"/>
+      <c r="K12" s="70"/>
     </row>
     <row r="13" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B13" s="32"/>
@@ -3405,7 +3401,7 @@
       <c r="H13" s="33"/>
       <c r="I13" s="34"/>
       <c r="J13" s="46"/>
-      <c r="K13" s="71"/>
+      <c r="K13" s="70"/>
     </row>
     <row r="14" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
@@ -3417,7 +3413,7 @@
       <c r="H14" s="33"/>
       <c r="I14" s="34"/>
       <c r="J14" s="46"/>
-      <c r="K14" s="71"/>
+      <c r="K14" s="70"/>
     </row>
     <row r="15" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B15" s="32"/>
@@ -3429,7 +3425,7 @@
       <c r="H15" s="33"/>
       <c r="I15" s="34"/>
       <c r="J15" s="46"/>
-      <c r="K15" s="71"/>
+      <c r="K15" s="70"/>
     </row>
     <row r="16" spans="1:212" x14ac:dyDescent="0.25">
       <c r="B16" s="32"/>
@@ -3441,7 +3437,7 @@
       <c r="H16" s="33"/>
       <c r="I16" s="34"/>
       <c r="J16" s="46"/>
-      <c r="K16" s="71"/>
+      <c r="K16" s="70"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="32"/>
@@ -3453,7 +3449,7 @@
       <c r="H17" s="33"/>
       <c r="I17" s="34"/>
       <c r="J17" s="46"/>
-      <c r="K17" s="71"/>
+      <c r="K17" s="70"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
@@ -3465,7 +3461,7 @@
       <c r="H18" s="33"/>
       <c r="I18" s="34"/>
       <c r="J18" s="46"/>
-      <c r="K18" s="71"/>
+      <c r="K18" s="70"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
@@ -3477,7 +3473,7 @@
       <c r="H19" s="33"/>
       <c r="I19" s="34"/>
       <c r="J19" s="46"/>
-      <c r="K19" s="71"/>
+      <c r="K19" s="70"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
@@ -3489,7 +3485,7 @@
       <c r="H20" s="33"/>
       <c r="I20" s="34"/>
       <c r="J20" s="46"/>
-      <c r="K20" s="71"/>
+      <c r="K20" s="70"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
@@ -3501,7 +3497,7 @@
       <c r="H21" s="33"/>
       <c r="I21" s="34"/>
       <c r="J21" s="46"/>
-      <c r="K21" s="71"/>
+      <c r="K21" s="70"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
@@ -3513,7 +3509,7 @@
       <c r="H22" s="33"/>
       <c r="I22" s="34"/>
       <c r="J22" s="46"/>
-      <c r="K22" s="71"/>
+      <c r="K22" s="70"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
@@ -3525,7 +3521,7 @@
       <c r="H23" s="33"/>
       <c r="I23" s="34"/>
       <c r="J23" s="46"/>
-      <c r="K23" s="71"/>
+      <c r="K23" s="70"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="32"/>
@@ -3537,7 +3533,7 @@
       <c r="H24" s="33"/>
       <c r="I24" s="34"/>
       <c r="J24" s="46"/>
-      <c r="K24" s="71"/>
+      <c r="K24" s="70"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="32"/>
@@ -3549,7 +3545,7 @@
       <c r="H25" s="33"/>
       <c r="I25" s="34"/>
       <c r="J25" s="46"/>
-      <c r="K25" s="71"/>
+      <c r="K25" s="70"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
@@ -3561,7 +3557,7 @@
       <c r="H26" s="33"/>
       <c r="I26" s="34"/>
       <c r="J26" s="46"/>
-      <c r="K26" s="71"/>
+      <c r="K26" s="70"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="32"/>
@@ -3573,7 +3569,7 @@
       <c r="H27" s="33"/>
       <c r="I27" s="34"/>
       <c r="J27" s="46"/>
-      <c r="K27" s="71"/>
+      <c r="K27" s="70"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="32"/>
@@ -3585,7 +3581,7 @@
       <c r="H28" s="33"/>
       <c r="I28" s="34"/>
       <c r="J28" s="46"/>
-      <c r="K28" s="71"/>
+      <c r="K28" s="70"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="32"/>
@@ -3597,7 +3593,7 @@
       <c r="H29" s="33"/>
       <c r="I29" s="34"/>
       <c r="J29" s="46"/>
-      <c r="K29" s="71"/>
+      <c r="K29" s="70"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="32"/>
@@ -3609,7 +3605,7 @@
       <c r="H30" s="33"/>
       <c r="I30" s="34"/>
       <c r="J30" s="46"/>
-      <c r="K30" s="71"/>
+      <c r="K30" s="70"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="32"/>
@@ -3621,7 +3617,7 @@
       <c r="H31" s="33"/>
       <c r="I31" s="34"/>
       <c r="J31" s="46"/>
-      <c r="K31" s="71"/>
+      <c r="K31" s="70"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
@@ -3633,7 +3629,7 @@
       <c r="H32" s="33"/>
       <c r="I32" s="34"/>
       <c r="J32" s="46"/>
-      <c r="K32" s="71"/>
+      <c r="K32" s="70"/>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
@@ -3645,7 +3641,7 @@
       <c r="H33" s="33"/>
       <c r="I33" s="34"/>
       <c r="J33" s="46"/>
-      <c r="K33" s="71"/>
+      <c r="K33" s="70"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="32"/>
@@ -3657,7 +3653,7 @@
       <c r="H34" s="33"/>
       <c r="I34" s="34"/>
       <c r="J34" s="46"/>
-      <c r="K34" s="71"/>
+      <c r="K34" s="70"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="32"/>
@@ -3669,7 +3665,7 @@
       <c r="H35" s="33"/>
       <c r="I35" s="34"/>
       <c r="J35" s="46"/>
-      <c r="K35" s="71"/>
+      <c r="K35" s="70"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
@@ -3681,7 +3677,7 @@
       <c r="H36" s="33"/>
       <c r="I36" s="34"/>
       <c r="J36" s="46"/>
-      <c r="K36" s="71"/>
+      <c r="K36" s="70"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="32"/>
@@ -3693,7 +3689,7 @@
       <c r="H37" s="33"/>
       <c r="I37" s="34"/>
       <c r="J37" s="46"/>
-      <c r="K37" s="71"/>
+      <c r="K37" s="70"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="32"/>
@@ -3705,7 +3701,7 @@
       <c r="H38" s="33"/>
       <c r="I38" s="34"/>
       <c r="J38" s="46"/>
-      <c r="K38" s="71"/>
+      <c r="K38" s="70"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="32"/>
@@ -3717,7 +3713,7 @@
       <c r="H39" s="33"/>
       <c r="I39" s="34"/>
       <c r="J39" s="46"/>
-      <c r="K39" s="71"/>
+      <c r="K39" s="70"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="32"/>
@@ -3729,7 +3725,7 @@
       <c r="H40" s="33"/>
       <c r="I40" s="34"/>
       <c r="J40" s="46"/>
-      <c r="K40" s="71"/>
+      <c r="K40" s="70"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="32"/>
@@ -3741,7 +3737,7 @@
       <c r="H41" s="33"/>
       <c r="I41" s="34"/>
       <c r="J41" s="46"/>
-      <c r="K41" s="71"/>
+      <c r="K41" s="70"/>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="32"/>
@@ -3753,7 +3749,7 @@
       <c r="H42" s="33"/>
       <c r="I42" s="34"/>
       <c r="J42" s="46"/>
-      <c r="K42" s="71"/>
+      <c r="K42" s="70"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
@@ -3765,7 +3761,7 @@
       <c r="H43" s="33"/>
       <c r="I43" s="34"/>
       <c r="J43" s="46"/>
-      <c r="K43" s="71"/>
+      <c r="K43" s="70"/>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
@@ -3777,7 +3773,7 @@
       <c r="H44" s="33"/>
       <c r="I44" s="34"/>
       <c r="J44" s="46"/>
-      <c r="K44" s="71"/>
+      <c r="K44" s="70"/>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
@@ -3789,7 +3785,7 @@
       <c r="H45" s="33"/>
       <c r="I45" s="34"/>
       <c r="J45" s="46"/>
-      <c r="K45" s="71"/>
+      <c r="K45" s="70"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="32"/>
@@ -3801,7 +3797,7 @@
       <c r="H46" s="33"/>
       <c r="I46" s="34"/>
       <c r="J46" s="46"/>
-      <c r="K46" s="71"/>
+      <c r="K46" s="70"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="32"/>
@@ -3813,7 +3809,7 @@
       <c r="H47" s="33"/>
       <c r="I47" s="34"/>
       <c r="J47" s="46"/>
-      <c r="K47" s="71"/>
+      <c r="K47" s="70"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="32"/>
@@ -3825,7 +3821,7 @@
       <c r="H48" s="33"/>
       <c r="I48" s="34"/>
       <c r="J48" s="46"/>
-      <c r="K48" s="71"/>
+      <c r="K48" s="70"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" s="32"/>
@@ -3837,7 +3833,7 @@
       <c r="H49" s="33"/>
       <c r="I49" s="34"/>
       <c r="J49" s="46"/>
-      <c r="K49" s="71"/>
+      <c r="K49" s="70"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="32"/>
@@ -3849,7 +3845,7 @@
       <c r="H50" s="33"/>
       <c r="I50" s="34"/>
       <c r="J50" s="46"/>
-      <c r="K50" s="71"/>
+      <c r="K50" s="70"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="32"/>
@@ -3861,7 +3857,7 @@
       <c r="H51" s="33"/>
       <c r="I51" s="34"/>
       <c r="J51" s="46"/>
-      <c r="K51" s="71"/>
+      <c r="K51" s="70"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" s="32"/>
@@ -3873,7 +3869,7 @@
       <c r="H52" s="33"/>
       <c r="I52" s="34"/>
       <c r="J52" s="46"/>
-      <c r="K52" s="71"/>
+      <c r="K52" s="70"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="32"/>
@@ -3885,7 +3881,7 @@
       <c r="H53" s="33"/>
       <c r="I53" s="34"/>
       <c r="J53" s="46"/>
-      <c r="K53" s="71"/>
+      <c r="K53" s="70"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" s="32"/>
@@ -3897,7 +3893,7 @@
       <c r="H54" s="33"/>
       <c r="I54" s="34"/>
       <c r="J54" s="46"/>
-      <c r="K54" s="71"/>
+      <c r="K54" s="70"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="32"/>
@@ -3909,7 +3905,7 @@
       <c r="H55" s="33"/>
       <c r="I55" s="34"/>
       <c r="J55" s="46"/>
-      <c r="K55" s="71"/>
+      <c r="K55" s="70"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="32"/>
@@ -3921,7 +3917,7 @@
       <c r="H56" s="33"/>
       <c r="I56" s="34"/>
       <c r="J56" s="46"/>
-      <c r="K56" s="71"/>
+      <c r="K56" s="70"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" s="32"/>
@@ -3933,7 +3929,7 @@
       <c r="H57" s="33"/>
       <c r="I57" s="34"/>
       <c r="J57" s="32"/>
-      <c r="K57" s="71"/>
+      <c r="K57" s="70"/>
     </row>
     <row r="1048575" spans="13:212" x14ac:dyDescent="0.25">
       <c r="M1048575" s="48"/>
@@ -4138,7 +4134,7 @@
       <c r="HD1048575" s="47"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vDsptiMRF8QIMLQpO3bZ1sESTVpUW1Hqfu69+NtC+0Eyc+2i6AnjikbLjmv8FUjGldUyruu0Rz2IoXDrFMQOYw==" saltValue="zXAfBtdGoej2q4pHRntN/Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="YWIsA9eqMSf0n4395nPBQFB6kbpB/9XAyDsLz81HLABM0BgId9KIUY8+qZjZE6Vc9XbY68ENfUbK5qidgd+EzA==" saltValue="rfZEofQ6OLarJIBXFqRE1Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="B4:F6"/>
     <mergeCell ref="G4:I6"/>
@@ -4172,7 +4168,7 @@
     <hyperlink ref="C7" r:id="rId7" location="fisheries" xr:uid="{F95149BA-1BB2-46CC-A86F-36B6AC4AFBA6}"/>
     <hyperlink ref="F7" r:id="rId8" location="discardReasons" display="Disc. reason" xr:uid="{4B127CA8-AB4F-43B9-B5B8-5A77A85A9028}"/>
     <hyperlink ref="L4" r:id="rId9" location="species" xr:uid="{0BBE03AC-0AAA-41DA-99E5-9DD325DC155B}"/>
-    <hyperlink ref="L5" r:id="rId10" location="catchUnits" display="Discard unit" xr:uid="{431CFE87-EEB6-4BEC-9E8B-1A482800044E}"/>
+    <hyperlink ref="L5" r:id="rId10" location="individualConditions" xr:uid="{431CFE87-EEB6-4BEC-9E8B-1A482800044E}"/>
     <hyperlink ref="D7" r:id="rId11" location="species" xr:uid="{6FA0C96E-7F47-464A-B5AC-18A928C06AB1}"/>
     <hyperlink ref="L6" r:id="rId12" location="raisings" xr:uid="{387C7B1D-B99F-4149-9A85-EE0666628CB0}"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Showing heading in metadata worksheets
</commit_message>
<xml_diff>
--- a/forms/Form-1DI.xlsx
+++ b/forms/Form-1DI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\bitbucket_workspaces\IOTC-ws\R libs\workflow\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1FB030-0581-4D2D-90F2-C8C9F03955A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FA571A-8536-4DCE-A739-78732538596F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -1476,7 +1476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>